<commit_message>
USDON and USDSTD reference date: bug fixed
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/USD/USD_YCSTDBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/USD/USD_YCSTDBootstrapping.xlsx
@@ -1250,14 +1250,14 @@
     <xf numFmtId="172" fontId="3" fillId="10" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1618,7 +1618,7 @@
       </c>
       <c r="I3" s="13">
         <f>_xll.qlSettingsEvaluationDate(Trigger)</f>
-        <v>42255</v>
+        <v>42318</v>
       </c>
       <c r="J3" s="83"/>
     </row>
@@ -1637,7 +1637,7 @@
       </c>
       <c r="I4" s="15">
         <f>_xll.qlCalendarAdvance(Calendar,Evaluationdate,"2D","F",,Trigger)</f>
-        <v>42257</v>
+        <v>42320</v>
       </c>
       <c r="J4" s="83"/>
     </row>
@@ -1647,9 +1647,7 @@
       <c r="C5" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="21">
-        <v>42255.629363425927</v>
-      </c>
+      <c r="D5" s="21"/>
       <c r="E5" s="83"/>
       <c r="G5" s="85"/>
       <c r="H5" s="14" t="s">
@@ -1779,8 +1777,8 @@
         <v>10</v>
       </c>
       <c r="D14" s="41" t="str">
-        <f>_xll.qlPiecewiseYieldCurve(D16,D17,Calendar,_xll.ohPack(USDSTD!W3:W71),,,,D18,D19,D20,Permanent,,ObjectOverwrite)</f>
-        <v>_USDSTD#0003</v>
+        <f>_xll.qlPiecewiseYieldCurve(D16,D17,LocalCalendar,_xll.ohPack(USDSTD!W3:W71),,,,D18,D19,D20,Permanent,,ObjectOverwrite)</f>
+        <v>_USDSTD#0002</v>
       </c>
       <c r="E14" s="42"/>
     </row>
@@ -1853,7 +1851,7 @@
       <c r="B22" s="23"/>
       <c r="C22" s="32">
         <f>_xll.qlTermStructureReferenceDate(YieldCurve_STD)</f>
-        <v>42255</v>
+        <v>42318</v>
       </c>
       <c r="D22" s="33">
         <f>_xll.qlYieldTSDiscount(YieldCurve_STD,C22,,Trigger)</f>
@@ -1865,11 +1863,11 @@
       <c r="B23" s="23"/>
       <c r="C23" s="34">
         <f>_xll.qlTermStructureMaxDate(YieldCurve_STD,Trigger)</f>
-        <v>53223</v>
+        <v>60584</v>
       </c>
       <c r="D23" s="35">
         <f>_xll.qlYieldTSDiscount(YieldCurve_STD,C23,,Trigger)</f>
-        <v>0.43380514110752189</v>
+        <v>0.25664810096502239</v>
       </c>
       <c r="E23" s="42"/>
     </row>
@@ -2088,12 +2086,12 @@
       </c>
       <c r="AC2" s="160">
         <f t="array" ref="AC2:AC71">_xll.qlPiecewiseYieldCurveData(YieldCurve_STD,Trigger)</f>
-        <v>2.8388778488116924E-3</v>
-      </c>
-      <c r="AE2" s="163" t="s">
+        <v>2.9402540924823879E-3</v>
+      </c>
+      <c r="AE2" s="164" t="s">
         <v>84</v>
       </c>
-      <c r="AF2" s="164"/>
+      <c r="AF2" s="165"/>
       <c r="AH2" s="161"/>
     </row>
     <row r="3" spans="1:34" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2111,7 +2109,7 @@
       <c r="F3" s="125"/>
       <c r="G3" s="114" t="str">
         <f>_xll.qlLibor(,Currency,C3,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0031e#0001</v>
+        <v>obj_00306#0001</v>
       </c>
       <c r="H3" s="122" t="str">
         <f t="shared" ref="H3:H11" si="0">Currency&amp;$B3&amp;"D"&amp;$H$1&amp;QuoteSuffix</f>
@@ -2120,7 +2118,7 @@
       <c r="I3" s="125"/>
       <c r="J3" s="115" t="str">
         <f>_xll.qlDepositRateHelper(,H3,G3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00323#0001</v>
+        <v>obj_0030a#0001</v>
       </c>
       <c r="K3" s="49"/>
       <c r="L3" s="66" t="str">
@@ -2129,7 +2127,7 @@
       </c>
       <c r="M3" s="133" t="str">
         <f>IF(ISBLANK(J3),"--",J3)</f>
-        <v>obj_00323#0001</v>
+        <v>obj_0030a#0001</v>
       </c>
       <c r="N3" s="147" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M3,Trigger),"--")</f>
@@ -2137,7 +2135,7 @@
       </c>
       <c r="O3" s="135">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M3,Trigger),"--")</f>
-        <v>2.7999999999999995E-3</v>
+        <v>2.8999999999999998E-3</v>
       </c>
       <c r="P3" s="134" t="b">
         <v>1</v>
@@ -2150,11 +2148,11 @@
       </c>
       <c r="S3" s="136">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M3,Trigger),"--")</f>
-        <v>42255</v>
+        <v>42318</v>
       </c>
       <c r="T3" s="136">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M3,Trigger),"--")</f>
-        <v>42256</v>
+        <v>42320</v>
       </c>
       <c r="V3" s="3" t="str">
         <f t="shared" ref="V3:V34" si="1">IFERROR(INDEX($L$3:$L$71,MATCH(X3,$N$3:$N$71,0),1),"")</f>
@@ -2162,7 +2160,7 @@
       </c>
       <c r="W3" s="3" t="str">
         <f t="array" ref="W3:W71">_xll.qlRateHelperSelection(_xll.ohFilter(RateHelpers,IncludeFlag),_xll.ohFilter(Priority,IncludeFlag),$AF$3,$AF$4,$AF$5,$AF$6,_xll.ohFilter(MinDistance,IncludeFlag),Trigger)</f>
-        <v>obj_00323</v>
+        <v>obj_0030a</v>
       </c>
       <c r="X3" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W3,Trigger),"")</f>
@@ -2170,7 +2168,7 @@
       </c>
       <c r="Y3" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W3,Trigger),"")</f>
-        <v>2.7999999999999995E-3</v>
+        <v>2.8999999999999998E-3</v>
       </c>
       <c r="Z3" s="105" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W3)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W3)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W3)),_xll.qlSwapRateHelperSpread($W3))</f>
@@ -2178,14 +2176,14 @@
       </c>
       <c r="AA3" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W3,Trigger),"")</f>
-        <v>42255</v>
+        <v>42318</v>
       </c>
       <c r="AB3" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W3,Trigger),"")</f>
-        <v>42256</v>
+        <v>42320</v>
       </c>
       <c r="AC3" s="68">
-        <v>2.8388778488116924E-3</v>
+        <v>2.9402540924823879E-3</v>
       </c>
       <c r="AE3" s="108" t="s">
         <v>85</v>
@@ -2210,7 +2208,7 @@
       <c r="F4" s="132"/>
       <c r="G4" s="55" t="str">
         <f>_xll.qlLibor(,Currency,C4,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00313#0001</v>
+        <v>obj_002fc#0001</v>
       </c>
       <c r="H4" s="158" t="str">
         <f t="shared" si="0"/>
@@ -2219,7 +2217,7 @@
       <c r="I4" s="132"/>
       <c r="J4" s="57" t="str">
         <f>_xll.qlFraRateHelper(,H4,"1D",G4,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00318#0001</v>
+        <v>obj_00307#0001</v>
       </c>
       <c r="K4" s="48"/>
       <c r="L4" s="9" t="str">
@@ -2228,7 +2226,7 @@
       </c>
       <c r="M4" s="95" t="str">
         <f t="shared" ref="M4:M11" si="3">IF(ISBLANK(J4),"--",J4)</f>
-        <v>obj_00318#0001</v>
+        <v>obj_00307#0001</v>
       </c>
       <c r="N4" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M4,Trigger),"--")</f>
@@ -2236,7 +2234,7 @@
       </c>
       <c r="O4" s="99">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M4,Trigger),"--")</f>
-        <v>2.7999999999999995E-3</v>
+        <v>2.8999999999999998E-3</v>
       </c>
       <c r="P4" s="98" t="b">
         <v>1</v>
@@ -2249,18 +2247,18 @@
       </c>
       <c r="S4" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M4,Trigger),"--")</f>
-        <v>42256</v>
+        <v>42320</v>
       </c>
       <c r="T4" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M4,Trigger),"--")</f>
-        <v>42257</v>
+        <v>42321</v>
       </c>
       <c r="V4" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Dp</v>
       </c>
       <c r="W4" s="3" t="str">
-        <v>obj_00318</v>
+        <v>obj_00307</v>
       </c>
       <c r="X4" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W4,Trigger),"")</f>
@@ -2268,7 +2266,7 @@
       </c>
       <c r="Y4" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W4,Trigger),"")</f>
-        <v>2.7999999999999995E-3</v>
+        <v>2.8999999999999998E-3</v>
       </c>
       <c r="Z4" s="105" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W4)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W4)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W4)),_xll.qlSwapRateHelperSpread($W4))</f>
@@ -2276,14 +2274,14 @@
       </c>
       <c r="AA4" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W4,Trigger),"")</f>
-        <v>42256</v>
+        <v>42320</v>
       </c>
       <c r="AB4" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W4,Trigger),"")</f>
-        <v>42257</v>
+        <v>42321</v>
       </c>
       <c r="AC4" s="68">
-        <v>2.8388778488016657E-3</v>
+        <v>2.9402580400256706E-3</v>
       </c>
       <c r="AE4" s="108" t="s">
         <v>86</v>
@@ -2308,7 +2306,7 @@
       <c r="F5" s="127"/>
       <c r="G5" s="6" t="str">
         <f>_xll.qlLibor(,Currency,C5,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0031c#0001</v>
+        <v>obj_00304#0001</v>
       </c>
       <c r="H5" s="124" t="str">
         <f t="shared" si="0"/>
@@ -2317,7 +2315,7 @@
       <c r="I5" s="127"/>
       <c r="J5" s="2" t="str">
         <f>_xll.qlFraRateHelper(,H5,"2D",G5,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0031f#0001</v>
+        <v>obj_00309#0001</v>
       </c>
       <c r="K5" s="48"/>
       <c r="L5" s="9" t="str">
@@ -2326,7 +2324,7 @@
       </c>
       <c r="M5" s="95" t="str">
         <f t="shared" si="3"/>
-        <v>obj_0031f#0001</v>
+        <v>obj_00309#0001</v>
       </c>
       <c r="N5" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M5,Trigger),"--")</f>
@@ -2334,7 +2332,7 @@
       </c>
       <c r="O5" s="99">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M5,Trigger),"--")</f>
-        <v>2.7999999999999995E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="P5" s="98" t="b">
         <v>1</v>
@@ -2347,18 +2345,18 @@
       </c>
       <c r="S5" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M5,Trigger),"--")</f>
-        <v>42257</v>
+        <v>42321</v>
       </c>
       <c r="T5" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M5,Trigger),"--")</f>
-        <v>42258</v>
+        <v>42324</v>
       </c>
       <c r="V5" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Dp</v>
       </c>
       <c r="W5" s="3" t="str">
-        <v>obj_0031f</v>
+        <v>obj_00309</v>
       </c>
       <c r="X5" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W5,Trigger),"")</f>
@@ -2366,7 +2364,7 @@
       </c>
       <c r="Y5" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W5,Trigger),"")</f>
-        <v>2.7999999999999995E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="Z5" s="105" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W5)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W5)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W5)),_xll.qlSwapRateHelperSpread($W5))</f>
@@ -2374,14 +2372,14 @@
       </c>
       <c r="AA5" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W5,Trigger),"")</f>
-        <v>42257</v>
+        <v>42321</v>
       </c>
       <c r="AB5" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W5,Trigger),"")</f>
-        <v>42258</v>
+        <v>42324</v>
       </c>
       <c r="AC5" s="68">
-        <v>2.8388778487858581E-3</v>
+        <v>2.9909433432465256E-3</v>
       </c>
       <c r="AD5" s="76"/>
       <c r="AE5" s="108" t="s">
@@ -2408,7 +2406,7 @@
       <c r="F6" s="126"/>
       <c r="G6" s="60" t="str">
         <f>_xll.qlLibor(,Currency,C6,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0031b#0001</v>
+        <v>obj_00303#0001</v>
       </c>
       <c r="H6" s="123" t="str">
         <f t="shared" si="0"/>
@@ -2417,7 +2415,7 @@
       <c r="I6" s="126"/>
       <c r="J6" s="62" t="str">
         <f>_xll.qlDepositRateHelper(,H6,G6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00320#0001</v>
+        <v>obj_00308#0001</v>
       </c>
       <c r="K6" s="48"/>
       <c r="L6" s="9" t="str">
@@ -2426,7 +2424,7 @@
       </c>
       <c r="M6" s="95" t="str">
         <f t="shared" si="3"/>
-        <v>obj_00320#0001</v>
+        <v>obj_00308#0001</v>
       </c>
       <c r="N6" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M6,Trigger),"--")</f>
@@ -2434,7 +2432,7 @@
       </c>
       <c r="O6" s="99">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M6,Trigger),"--")</f>
-        <v>1.5399999999999999E-3</v>
+        <v>1.5560000000000001E-3</v>
       </c>
       <c r="P6" s="98" t="b">
         <v>1</v>
@@ -2447,18 +2445,18 @@
       </c>
       <c r="S6" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M6,Trigger),"--")</f>
-        <v>42257</v>
+        <v>42320</v>
       </c>
       <c r="T6" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M6,Trigger),"--")</f>
-        <v>42264</v>
+        <v>42327</v>
       </c>
       <c r="V6" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Dp</v>
       </c>
       <c r="W6" s="3" t="str">
-        <v>obj_00320</v>
+        <v>obj_00308</v>
       </c>
       <c r="X6" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W6,Trigger),"")</f>
@@ -2466,7 +2464,7 @@
       </c>
       <c r="Y6" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W6,Trigger),"")</f>
-        <v>1.5399999999999999E-3</v>
+        <v>1.5560000000000001E-3</v>
       </c>
       <c r="Z6" s="105" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W6)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W6)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W6)),_xll.qlSwapRateHelperSpread($W6))</f>
@@ -2474,14 +2472,14 @@
       </c>
       <c r="AA6" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W6,Trigger),"")</f>
-        <v>42257</v>
+        <v>42320</v>
       </c>
       <c r="AB6" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W6,Trigger),"")</f>
-        <v>42264</v>
+        <v>42327</v>
       </c>
       <c r="AC6" s="68">
-        <v>1.8452571423215789E-3</v>
+        <v>1.8804021006482438E-3</v>
       </c>
       <c r="AE6" s="108" t="s">
         <v>88</v>
@@ -2507,7 +2505,7 @@
       <c r="F7" s="126"/>
       <c r="G7" s="60" t="str">
         <f>_xll.qlLibor(,Currency,C7,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0031a#0001</v>
+        <v>obj_00302#0001</v>
       </c>
       <c r="H7" s="123" t="str">
         <f t="shared" si="0"/>
@@ -2516,7 +2514,7 @@
       <c r="I7" s="126"/>
       <c r="J7" s="62" t="str">
         <f>_xll.qlDepositRateHelper(,H7,G7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00321#0001</v>
+        <v>obj_0030c#0001</v>
       </c>
       <c r="K7" s="48"/>
       <c r="L7" s="9" t="str">
@@ -2525,7 +2523,7 @@
       </c>
       <c r="M7" s="95" t="str">
         <f t="shared" si="3"/>
-        <v>obj_00321#0001</v>
+        <v>obj_0030c#0001</v>
       </c>
       <c r="N7" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M7,Trigger),"--")</f>
@@ -2533,7 +2531,7 @@
       </c>
       <c r="O7" s="99">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M7,Trigger),"--")</f>
-        <v>2.0299999999999997E-3</v>
+        <v>1.97E-3</v>
       </c>
       <c r="P7" s="98" t="b">
         <v>1</v>
@@ -2546,18 +2544,18 @@
       </c>
       <c r="S7" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M7,Trigger),"--")</f>
-        <v>42257</v>
+        <v>42320</v>
       </c>
       <c r="T7" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M7,Trigger),"--")</f>
-        <v>42290</v>
+        <v>42352</v>
       </c>
       <c r="V7" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Dp</v>
       </c>
       <c r="W7" s="3" t="str">
-        <v>obj_00321</v>
+        <v>obj_0030c</v>
       </c>
       <c r="X7" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W7,Trigger),"")</f>
@@ -2565,7 +2563,7 @@
       </c>
       <c r="Y7" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W7,Trigger),"")</f>
-        <v>2.0299999999999997E-3</v>
+        <v>1.97E-3</v>
       </c>
       <c r="Z7" s="105" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W7)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W7)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W7)),_xll.qlSwapRateHelperSpread($W7))</f>
@@ -2573,14 +2571,14 @@
       </c>
       <c r="AA7" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W7,Trigger),"")</f>
-        <v>42257</v>
+        <v>42320</v>
       </c>
       <c r="AB7" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W7,Trigger),"")</f>
-        <v>42290</v>
+        <v>42352</v>
       </c>
       <c r="AC7" s="68">
-        <v>2.1026243919511048E-3</v>
+        <v>2.052660830115613E-3</v>
       </c>
       <c r="AH7" s="161"/>
     </row>
@@ -2600,7 +2598,7 @@
       <c r="F8" s="126"/>
       <c r="G8" s="60" t="str">
         <f>_xll.qlLibor(,Currency,C8,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0031d#0001</v>
+        <v>obj_00305#0001</v>
       </c>
       <c r="H8" s="123" t="str">
         <f t="shared" si="0"/>
@@ -2609,7 +2607,7 @@
       <c r="I8" s="126"/>
       <c r="J8" s="62" t="str">
         <f>_xll.qlDepositRateHelper(,H8,G8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00322#0001</v>
+        <v>obj_0030b#0001</v>
       </c>
       <c r="K8" s="48"/>
       <c r="L8" s="9" t="str">
@@ -2618,7 +2616,7 @@
       </c>
       <c r="M8" s="95" t="str">
         <f t="shared" si="3"/>
-        <v>obj_00322#0001</v>
+        <v>obj_0030b#0001</v>
       </c>
       <c r="N8" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M8,Trigger),"--")</f>
@@ -2626,7 +2624,7 @@
       </c>
       <c r="O8" s="99">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M8,Trigger),"--")</f>
-        <v>2.6855E-3</v>
+        <v>2.725E-3</v>
       </c>
       <c r="P8" s="98" t="b">
         <v>1</v>
@@ -2639,18 +2637,18 @@
       </c>
       <c r="S8" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M8,Trigger),"--")</f>
-        <v>42257</v>
+        <v>42320</v>
       </c>
       <c r="T8" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M8,Trigger),"--")</f>
-        <v>42318</v>
+        <v>42381</v>
       </c>
       <c r="V8" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Dp</v>
       </c>
       <c r="W8" s="3" t="str">
-        <v>obj_00322</v>
+        <v>obj_0030b</v>
       </c>
       <c r="X8" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W8,Trigger),"")</f>
@@ -2658,7 +2656,7 @@
       </c>
       <c r="Y8" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W8,Trigger),"")</f>
-        <v>2.6855E-3</v>
+        <v>2.725E-3</v>
       </c>
       <c r="Z8" s="105" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W8)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W8)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W8)),_xll.qlSwapRateHelperSpread($W8))</f>
@@ -2666,14 +2664,14 @@
       </c>
       <c r="AA8" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W8,Trigger),"")</f>
-        <v>42257</v>
+        <v>42320</v>
       </c>
       <c r="AB8" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W8,Trigger),"")</f>
-        <v>42318</v>
+        <v>42381</v>
       </c>
       <c r="AC8" s="68">
-        <v>2.725884019396098E-3</v>
+        <v>2.7678617725453596E-3</v>
       </c>
       <c r="AH8" s="161"/>
     </row>
@@ -2693,7 +2691,7 @@
       <c r="F9" s="126"/>
       <c r="G9" s="60" t="str">
         <f>_xll.qlLibor(,Currency,C9,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00314#0001</v>
+        <v>obj_002fd#0001</v>
       </c>
       <c r="H9" s="123" t="str">
         <f t="shared" si="0"/>
@@ -2702,7 +2700,7 @@
       <c r="I9" s="126"/>
       <c r="J9" s="62" t="str">
         <f>_xll.qlDepositRateHelper(,H9,G9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00315#0001</v>
+        <v>obj_002fe#0001</v>
       </c>
       <c r="K9" s="48"/>
       <c r="L9" s="9" t="str">
@@ -2711,7 +2709,7 @@
       </c>
       <c r="M9" s="95" t="str">
         <f t="shared" si="3"/>
-        <v>obj_00315#0001</v>
+        <v>obj_002fe#0001</v>
       </c>
       <c r="N9" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M9,Trigger),"--")</f>
@@ -2719,7 +2717,7 @@
       </c>
       <c r="O9" s="99">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M9,Trigger),"--")</f>
-        <v>3.3199999999999996E-3</v>
+        <v>3.5560000000000001E-3</v>
       </c>
       <c r="P9" s="98" t="b">
         <v>1</v>
@@ -2732,41 +2730,41 @@
       </c>
       <c r="S9" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M9,Trigger),"--")</f>
-        <v>42257</v>
+        <v>42320</v>
       </c>
       <c r="T9" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M9,Trigger),"--")</f>
-        <v>42348</v>
+        <v>42412</v>
       </c>
       <c r="V9" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>FUT</v>
+        <v>Dp</v>
       </c>
       <c r="W9" s="3" t="str">
-        <v>obj_00335</v>
+        <v>obj_002fe</v>
       </c>
       <c r="X9" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W9,Trigger),"")</f>
-        <v>USDFUT3MU5_Quote</v>
+        <v>USD3MD_Quote</v>
       </c>
       <c r="Y9" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W9,Trigger),"")</f>
-        <v>3.4370538179827846E-3</v>
-      </c>
-      <c r="Z9" s="105">
+        <v>3.5560000000000001E-3</v>
+      </c>
+      <c r="Z9" s="105" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W9)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W9)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W9)),_xll.qlSwapRateHelperSpread($W9))</f>
-        <v>4.4618201719769934E-7</v>
+        <v/>
       </c>
       <c r="AA9" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W9,Trigger),"")</f>
-        <v>42263</v>
+        <v>42320</v>
       </c>
       <c r="AB9" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W9,Trigger),"")</f>
-        <v>42354</v>
+        <v>42412</v>
       </c>
       <c r="AC9" s="68">
-        <v>3.3642945370357595E-3</v>
+        <v>3.589634702329533E-3</v>
       </c>
       <c r="AH9" s="161"/>
     </row>
@@ -2786,7 +2784,7 @@
       <c r="F10" s="126"/>
       <c r="G10" s="60" t="str">
         <f>_xll.qlLibor(,Currency,C10,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00316#0001</v>
+        <v>obj_002ff#0001</v>
       </c>
       <c r="H10" s="123" t="str">
         <f t="shared" si="0"/>
@@ -2833,7 +2831,7 @@
         <v>FUT</v>
       </c>
       <c r="W10" s="3" t="str">
-        <v>obj_00334</v>
+        <v>obj_0031d</v>
       </c>
       <c r="X10" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W10,Trigger),"")</f>
@@ -2841,11 +2839,11 @@
       </c>
       <c r="Y10" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W10,Trigger),"")</f>
-        <v>4.8168832263151308E-3</v>
+        <v>4.3729641797705821E-3</v>
       </c>
       <c r="Z10" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W10)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W10)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W10)),_xll.qlSwapRateHelperSpread($W10))</f>
-        <v>8.1167736848374994E-6</v>
+        <v>2.0358202294357524E-6</v>
       </c>
       <c r="AA10" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W10,Trigger),"")</f>
@@ -2856,7 +2854,7 @@
         <v>42445</v>
       </c>
       <c r="AC10" s="68">
-        <v>4.0906273241313488E-3</v>
+        <v>3.770986716006456E-3</v>
       </c>
       <c r="AH10" s="161"/>
     </row>
@@ -2876,7 +2874,7 @@
       <c r="F11" s="127"/>
       <c r="G11" s="6" t="str">
         <f>_xll.qlLibor(,Currency,C11,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00317#0001</v>
+        <v>obj_00300#0001</v>
       </c>
       <c r="H11" s="124" t="str">
         <f t="shared" si="0"/>
@@ -2923,7 +2921,7 @@
         <v>FUT</v>
       </c>
       <c r="W11" s="3" t="str">
-        <v>obj_00339</v>
+        <v>obj_00321</v>
       </c>
       <c r="X11" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W11,Trigger),"")</f>
@@ -2931,11 +2929,11 @@
       </c>
       <c r="Y11" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W11,Trigger),"")</f>
-        <v>6.104405001778699E-3</v>
+        <v>6.0648182583541007E-3</v>
       </c>
       <c r="Z11" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W11)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W11)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W11)),_xll.qlSwapRateHelperSpread($W11))</f>
-        <v>2.0594998221237348E-5</v>
+        <v>1.0181741645951506E-5</v>
       </c>
       <c r="AA11" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W11,Trigger),"")</f>
@@ -2946,7 +2944,7 @@
         <v>42537</v>
       </c>
       <c r="AC11" s="68">
-        <v>4.7736909427556172E-3</v>
+        <v>4.7679914916027759E-3</v>
       </c>
       <c r="AH11" s="161"/>
     </row>
@@ -2969,15 +2967,15 @@
       </c>
       <c r="M12" s="133" t="str">
         <f t="shared" ref="M12:M33" si="6">IF(ISBLANK(J14),"--",J14)</f>
-        <v>obj_00335#0001</v>
+        <v>obj_0031f#0001</v>
       </c>
       <c r="N12" s="147" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M12,Trigger),"--")</f>
-        <v>USDFUT3MU5_Quote</v>
+        <v>USDFUT3MX5_Quote</v>
       </c>
       <c r="O12" s="152">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M12,Trigger),"--")</f>
-        <v>99.65625</v>
+        <v>99.631249999999994</v>
       </c>
       <c r="P12" s="134" t="b">
         <v>1</v>
@@ -2990,18 +2988,18 @@
       </c>
       <c r="S12" s="136">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M12,Trigger),"--")</f>
-        <v>42263</v>
+        <v>42326</v>
       </c>
       <c r="T12" s="136">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M12,Trigger),"--")</f>
-        <v>42354</v>
+        <v>42418</v>
       </c>
       <c r="V12" s="3" t="str">
         <f t="shared" si="1"/>
         <v>FUT</v>
       </c>
       <c r="W12" s="3" t="str">
-        <v>obj_0033a</v>
+        <v>obj_00322</v>
       </c>
       <c r="X12" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W12,Trigger),"")</f>
@@ -3009,11 +3007,11 @@
       </c>
       <c r="Y12" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W12,Trigger),"")</f>
-        <v>7.637386173847089E-3</v>
+        <v>7.602558496357415E-3</v>
       </c>
       <c r="Z12" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W12)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W12)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W12)),_xll.qlSwapRateHelperSpread($W12))</f>
-        <v>3.7613826152898039E-5</v>
+        <v>2.2441503642577717E-5</v>
       </c>
       <c r="AA12" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W12,Trigger),"")</f>
@@ -3024,7 +3022,7 @@
         <v>42628</v>
       </c>
       <c r="AC12" s="68">
-        <v>5.4987263630684197E-3</v>
+        <v>5.6307143072360484E-3</v>
       </c>
       <c r="AH12" s="161"/>
     </row>
@@ -3060,15 +3058,15 @@
       </c>
       <c r="M13" s="95" t="str">
         <f t="shared" si="6"/>
-        <v>obj_00338#0001</v>
+        <v>obj_0031d#0001</v>
       </c>
       <c r="N13" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M13,Trigger),"--")</f>
-        <v>USDFUT3MV5_Quote</v>
+        <v>USDFUT3MZ5_Quote</v>
       </c>
       <c r="O13" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M13,Trigger),"--")</f>
-        <v>99.592500000000001</v>
+        <v>99.5625</v>
       </c>
       <c r="P13" s="98" t="b">
         <v>1</v>
@@ -3081,18 +3079,18 @@
       </c>
       <c r="S13" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M13,Trigger),"--")</f>
-        <v>42298</v>
+        <v>42354</v>
       </c>
       <c r="T13" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M13,Trigger),"--")</f>
-        <v>42390</v>
+        <v>42445</v>
       </c>
       <c r="V13" s="3" t="str">
         <f t="shared" si="1"/>
         <v>FUT</v>
       </c>
       <c r="W13" s="3" t="str">
-        <v>obj_0033b</v>
+        <v>obj_00323</v>
       </c>
       <c r="X13" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W13,Trigger),"")</f>
@@ -3100,11 +3098,11 @@
       </c>
       <c r="Y13" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W13,Trigger),"")</f>
-        <v>9.3642442569190649E-3</v>
+        <v>9.3349948777573678E-3</v>
       </c>
       <c r="Z13" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W13)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W13)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W13)),_xll.qlSwapRateHelperSpread($W13))</f>
-        <v>6.0755743080840787E-5</v>
+        <v>4.0005122242654754E-5</v>
       </c>
       <c r="AA13" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W13,Trigger),"")</f>
@@ -3115,7 +3113,7 @@
         <v>42725</v>
       </c>
       <c r="AC13" s="68">
-        <v>6.3106647996998833E-3</v>
+        <v>6.5285594706942767E-3</v>
       </c>
       <c r="AH13" s="161"/>
     </row>
@@ -3128,7 +3126,7 @@
       </c>
       <c r="C14" s="56" t="str">
         <f>_xll.qlIMMNextCode(Evaluationdate-1,B14,Trigger)</f>
-        <v>U5</v>
+        <v>X5</v>
       </c>
       <c r="D14" s="132"/>
       <c r="E14" s="132"/>
@@ -3139,15 +3137,15 @@
       </c>
       <c r="H14" s="119" t="str">
         <f t="shared" ref="H14:H35" si="8">Currency&amp;"FUT"&amp;$G$1&amp;$C14&amp;QuoteSuffix</f>
-        <v>USDFUT3MU5_Quote</v>
+        <v>USDFUT3MX5_Quote</v>
       </c>
       <c r="I14" s="119" t="str">
         <f t="shared" ref="I14:I35" si="9">Currency&amp;"FUT"&amp;$G$1&amp;$C14&amp;"ConvAdj"&amp;QuoteSuffix</f>
-        <v>USDFUT3MU5ConvAdj_Quote</v>
+        <v>USDFUT3MX5ConvAdj_Quote</v>
       </c>
       <c r="J14" s="57" t="str">
         <f>_xll.qlFuturesRateHelper(,H14,$H$12,C14,G14,I14,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00335#0001</v>
+        <v>obj_0031f#0001</v>
       </c>
       <c r="K14" s="48"/>
       <c r="L14" s="9" t="str">
@@ -3156,15 +3154,15 @@
       </c>
       <c r="M14" s="95" t="str">
         <f t="shared" si="6"/>
-        <v>obj_00337#0001</v>
+        <v>obj_00320#0001</v>
       </c>
       <c r="N14" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M14,Trigger),"--")</f>
-        <v>USDFUT3MX5_Quote</v>
+        <v>USDFUT3MF6_Quote</v>
       </c>
       <c r="O14" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M14,Trigger),"--")</f>
-        <v>99.557500000000005</v>
+        <v>99.492500000000007</v>
       </c>
       <c r="P14" s="98" t="b">
         <v>1</v>
@@ -3177,18 +3175,18 @@
       </c>
       <c r="S14" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M14,Trigger),"--")</f>
-        <v>42326</v>
+        <v>42389</v>
       </c>
       <c r="T14" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M14,Trigger),"--")</f>
-        <v>42418</v>
+        <v>42480</v>
       </c>
       <c r="V14" s="3" t="str">
         <f t="shared" si="1"/>
         <v>FUT</v>
       </c>
       <c r="W14" s="3" t="str">
-        <v>obj_0033c</v>
+        <v>obj_00324</v>
       </c>
       <c r="X14" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W14,Trigger),"")</f>
@@ -3196,11 +3194,11 @@
       </c>
       <c r="Y14" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W14,Trigger),"")</f>
-        <v>1.1188300827818833E-2</v>
+        <v>1.1064680754560763E-2</v>
       </c>
       <c r="Z14" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W14)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W14)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W14)),_xll.qlSwapRateHelperSpread($W14))</f>
-        <v>8.6699172181091194E-5</v>
+        <v>6.0319245439177848E-5</v>
       </c>
       <c r="AA14" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W14,Trigger),"")</f>
@@ -3211,7 +3209,7 @@
         <v>42815</v>
       </c>
       <c r="AC14" s="68">
-        <v>7.1169995551010759E-3</v>
+        <v>7.375014000973029E-3</v>
       </c>
       <c r="AH14" s="161"/>
     </row>
@@ -3224,7 +3222,7 @@
       </c>
       <c r="C15" s="61" t="str">
         <f>_xll.qlIMMNextCode(C14,B15,Trigger)</f>
-        <v>V5</v>
+        <v>Z5</v>
       </c>
       <c r="D15" s="126"/>
       <c r="E15" s="126"/>
@@ -3235,15 +3233,15 @@
       </c>
       <c r="H15" s="120" t="str">
         <f t="shared" si="8"/>
-        <v>USDFUT3MV5_Quote</v>
+        <v>USDFUT3MZ5_Quote</v>
       </c>
       <c r="I15" s="120" t="str">
         <f t="shared" si="9"/>
-        <v>USDFUT3MV5ConvAdj_Quote</v>
+        <v>USDFUT3MZ5ConvAdj_Quote</v>
       </c>
       <c r="J15" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H15,$H$12,C15,G15,I15,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00338#0001</v>
+        <v>obj_0031d#0001</v>
       </c>
       <c r="K15" s="48"/>
       <c r="L15" s="9" t="str">
@@ -3252,15 +3250,15 @@
       </c>
       <c r="M15" s="95" t="str">
         <f t="shared" si="6"/>
-        <v>obj_00334#0001</v>
+        <v>obj_0031e#0001</v>
       </c>
       <c r="N15" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M15,Trigger),"--")</f>
-        <v>USDFUT3MZ5_Quote</v>
+        <v>USDFUT3MG6_Quote</v>
       </c>
       <c r="O15" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M15,Trigger),"--")</f>
-        <v>99.517499999999998</v>
+        <v>99.4375</v>
       </c>
       <c r="P15" s="98" t="b">
         <v>1</v>
@@ -3273,41 +3271,41 @@
       </c>
       <c r="S15" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M15,Trigger),"--")</f>
-        <v>42354</v>
+        <v>42417</v>
       </c>
       <c r="T15" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M15,Trigger),"--")</f>
-        <v>42445</v>
+        <v>42507</v>
       </c>
       <c r="V15" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>Sw</v>
+        <v>FUT</v>
       </c>
       <c r="W15" s="3" t="str">
-        <v>obj_00319</v>
+        <v>obj_00325</v>
       </c>
       <c r="X15" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W15,Trigger),"")</f>
-        <v>USDAM3L2Y_Quote</v>
+        <v>USDFUT3MH7_Quote</v>
       </c>
       <c r="Y15" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W15,Trigger),"")</f>
-        <v>8.539999999999999E-3</v>
+        <v>1.2641861312049179E-2</v>
       </c>
       <c r="Z15" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W15)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W15)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W15)),_xll.qlSwapRateHelperSpread($W15))</f>
-        <v>0</v>
+        <v>8.3138687950917617E-5</v>
       </c>
       <c r="AA15" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W15,Trigger),"")</f>
-        <v>42257</v>
+        <v>42809</v>
       </c>
       <c r="AB15" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W15,Trigger),"")</f>
-        <v>42989</v>
+        <v>42901</v>
       </c>
       <c r="AC15" s="68">
-        <v>8.6070054521104663E-3</v>
+        <v>8.1830679106953581E-3</v>
       </c>
       <c r="AH15" s="161"/>
     </row>
@@ -3320,7 +3318,7 @@
       </c>
       <c r="C16" s="61" t="str">
         <f>_xll.qlIMMNextCode(C15,B16,Trigger)</f>
-        <v>X5</v>
+        <v>F6</v>
       </c>
       <c r="D16" s="126"/>
       <c r="E16" s="126"/>
@@ -3331,15 +3329,15 @@
       </c>
       <c r="H16" s="120" t="str">
         <f t="shared" si="8"/>
-        <v>USDFUT3MX5_Quote</v>
+        <v>USDFUT3MF6_Quote</v>
       </c>
       <c r="I16" s="120" t="str">
         <f t="shared" si="9"/>
-        <v>USDFUT3MX5ConvAdj_Quote</v>
+        <v>USDFUT3MF6ConvAdj_Quote</v>
       </c>
       <c r="J16" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H16,$H$12,C16,G16,I16,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00337#0001</v>
+        <v>obj_00320#0001</v>
       </c>
       <c r="K16" s="48"/>
       <c r="L16" s="9" t="str">
@@ -3348,15 +3346,15 @@
       </c>
       <c r="M16" s="95" t="str">
         <f t="shared" si="6"/>
-        <v>obj_00336#0001</v>
+        <v>obj_00321#0001</v>
       </c>
       <c r="N16" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M16,Trigger),"--")</f>
-        <v>USDFUT3MF6_Quote</v>
+        <v>USDFUT3MH6_Quote</v>
       </c>
       <c r="O16" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M16,Trigger),"--")</f>
-        <v>99.477499999999992</v>
+        <v>99.392499999999998</v>
       </c>
       <c r="P16" s="98" t="b">
         <v>1</v>
@@ -3369,26 +3367,26 @@
       </c>
       <c r="S16" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M16,Trigger),"--")</f>
-        <v>42389</v>
+        <v>42445</v>
       </c>
       <c r="T16" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M16,Trigger),"--")</f>
-        <v>42480</v>
+        <v>42537</v>
       </c>
       <c r="V16" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Sw</v>
       </c>
       <c r="W16" s="3" t="str">
-        <v>obj_0032c</v>
+        <v>obj_00301</v>
       </c>
       <c r="X16" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W16,Trigger),"")</f>
-        <v>USDAM3L3Y_Quote</v>
+        <v>USDAM3L2Y_Quote</v>
       </c>
       <c r="Y16" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W16,Trigger),"")</f>
-        <v>1.1339999999999999E-2</v>
+        <v>9.4699999999999993E-3</v>
       </c>
       <c r="Z16" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W16)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W16)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W16)),_xll.qlSwapRateHelperSpread($W16))</f>
@@ -3396,14 +3394,14 @@
       </c>
       <c r="AA16" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W16,Trigger),"")</f>
-        <v>42257</v>
+        <v>42321</v>
       </c>
       <c r="AB16" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W16,Trigger),"")</f>
-        <v>43353</v>
+        <v>43052</v>
       </c>
       <c r="AC16" s="68">
-        <v>1.1452871785900676E-2</v>
+        <v>9.5447881453849231E-3</v>
       </c>
       <c r="AH16" s="161"/>
     </row>
@@ -3416,7 +3414,7 @@
       </c>
       <c r="C17" s="61" t="str">
         <f>_xll.qlIMMNextCode(C16,B17,Trigger)</f>
-        <v>Z5</v>
+        <v>G6</v>
       </c>
       <c r="D17" s="126"/>
       <c r="E17" s="126"/>
@@ -3427,15 +3425,15 @@
       </c>
       <c r="H17" s="120" t="str">
         <f t="shared" si="8"/>
-        <v>USDFUT3MZ5_Quote</v>
+        <v>USDFUT3MG6_Quote</v>
       </c>
       <c r="I17" s="120" t="str">
         <f t="shared" si="9"/>
-        <v>USDFUT3MZ5ConvAdj_Quote</v>
+        <v>USDFUT3MG6ConvAdj_Quote</v>
       </c>
       <c r="J17" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H17,$H$12,C17,G17,I17,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00334#0001</v>
+        <v>obj_0031e#0001</v>
       </c>
       <c r="K17" s="48"/>
       <c r="L17" s="9" t="str">
@@ -3444,15 +3442,15 @@
       </c>
       <c r="M17" s="95" t="str">
         <f t="shared" si="6"/>
-        <v>obj_00339#0001</v>
+        <v>obj_00322#0001</v>
       </c>
       <c r="N17" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M17,Trigger),"--")</f>
-        <v>USDFUT3MH6_Quote</v>
+        <v>USDFUT3MM6_Quote</v>
       </c>
       <c r="O17" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M17,Trigger),"--")</f>
-        <v>99.387500000000003</v>
+        <v>99.237499999999997</v>
       </c>
       <c r="P17" s="98" t="b">
         <v>1</v>
@@ -3465,26 +3463,26 @@
       </c>
       <c r="S17" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M17,Trigger),"--")</f>
-        <v>42445</v>
+        <v>42536</v>
       </c>
       <c r="T17" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M17,Trigger),"--")</f>
-        <v>42537</v>
+        <v>42628</v>
       </c>
       <c r="V17" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Sw</v>
       </c>
       <c r="W17" s="3" t="str">
-        <v>obj_00329</v>
+        <v>obj_0030e</v>
       </c>
       <c r="X17" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W17,Trigger),"")</f>
-        <v>USDAM3L4Y_Quote</v>
+        <v>USDAM3L3Y_Quote</v>
       </c>
       <c r="Y17" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W17,Trigger),"")</f>
-        <v>1.3729999999999999E-2</v>
+        <v>1.2359999999999999E-2</v>
       </c>
       <c r="Z17" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W17)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W17)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W17)),_xll.qlSwapRateHelperSpread($W17))</f>
@@ -3492,14 +3490,14 @@
       </c>
       <c r="AA17" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W17,Trigger),"")</f>
-        <v>42257</v>
+        <v>42321</v>
       </c>
       <c r="AB17" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W17,Trigger),"")</f>
-        <v>43718</v>
+        <v>43417</v>
       </c>
       <c r="AC17" s="68">
-        <v>1.3895081479232093E-2</v>
+        <v>1.2478454077713726E-2</v>
       </c>
       <c r="AH17" s="161"/>
     </row>
@@ -3512,7 +3510,7 @@
       </c>
       <c r="C18" s="8" t="str">
         <f>_xll.qlIMMNextCode(C17,B18,Trigger)</f>
-        <v>F6</v>
+        <v>H6</v>
       </c>
       <c r="D18" s="127"/>
       <c r="E18" s="127"/>
@@ -3523,15 +3521,15 @@
       </c>
       <c r="H18" s="121" t="str">
         <f t="shared" si="8"/>
-        <v>USDFUT3MF6_Quote</v>
+        <v>USDFUT3MH6_Quote</v>
       </c>
       <c r="I18" s="121" t="str">
         <f t="shared" si="9"/>
-        <v>USDFUT3MF6ConvAdj_Quote</v>
+        <v>USDFUT3MH6ConvAdj_Quote</v>
       </c>
       <c r="J18" s="2" t="str">
         <f>_xll.qlFuturesRateHelper(,H18,$H$12,C18,G18,I18,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00336#0001</v>
+        <v>obj_00321#0001</v>
       </c>
       <c r="K18" s="48"/>
       <c r="L18" s="9" t="str">
@@ -3540,15 +3538,15 @@
       </c>
       <c r="M18" s="95" t="str">
         <f t="shared" si="6"/>
-        <v>obj_0033a#0001</v>
+        <v>obj_00323#0001</v>
       </c>
       <c r="N18" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M18,Trigger),"--")</f>
-        <v>USDFUT3MM6_Quote</v>
+        <v>USDFUT3MU6_Quote</v>
       </c>
       <c r="O18" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M18,Trigger),"--")</f>
-        <v>99.232500000000002</v>
+        <v>99.0625</v>
       </c>
       <c r="P18" s="98" t="b">
         <v>1</v>
@@ -3561,26 +3559,26 @@
       </c>
       <c r="S18" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M18,Trigger),"--")</f>
-        <v>42536</v>
+        <v>42634</v>
       </c>
       <c r="T18" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M18,Trigger),"--")</f>
-        <v>42628</v>
+        <v>42725</v>
       </c>
       <c r="V18" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Sw</v>
       </c>
       <c r="W18" s="3" t="str">
-        <v>obj_0032b</v>
+        <v>obj_0030d</v>
       </c>
       <c r="X18" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W18,Trigger),"")</f>
-        <v>USDAM3L5Y_Quote</v>
+        <v>USDAM3L4Y_Quote</v>
       </c>
       <c r="Y18" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W18,Trigger),"")</f>
-        <v>1.5769999999999999E-2</v>
+        <v>1.4649999999999998E-2</v>
       </c>
       <c r="Z18" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W18)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W18)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W18)),_xll.qlSwapRateHelperSpread($W18))</f>
@@ -3588,14 +3586,14 @@
       </c>
       <c r="AA18" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W18,Trigger),"")</f>
-        <v>42257</v>
+        <v>42321</v>
       </c>
       <c r="AB18" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W18,Trigger),"")</f>
-        <v>44084</v>
+        <v>43782</v>
       </c>
       <c r="AC18" s="68">
-        <v>1.5994515444885553E-2</v>
+        <v>1.4817043325496866E-2</v>
       </c>
       <c r="AH18" s="161"/>
     </row>
@@ -3608,7 +3606,7 @@
       </c>
       <c r="C19" s="61" t="str">
         <f>_xll.qlIMMNextCode(C18,B19,Trigger)</f>
-        <v>H6</v>
+        <v>M6</v>
       </c>
       <c r="D19" s="126"/>
       <c r="E19" s="126"/>
@@ -3619,15 +3617,15 @@
       </c>
       <c r="H19" s="120" t="str">
         <f t="shared" si="8"/>
-        <v>USDFUT3MH6_Quote</v>
+        <v>USDFUT3MM6_Quote</v>
       </c>
       <c r="I19" s="120" t="str">
         <f t="shared" si="9"/>
-        <v>USDFUT3MH6ConvAdj_Quote</v>
+        <v>USDFUT3MM6ConvAdj_Quote</v>
       </c>
       <c r="J19" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H19,$H$12,C19,G19,I19,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00339#0001</v>
+        <v>obj_00322#0001</v>
       </c>
       <c r="K19" s="48"/>
       <c r="L19" s="9" t="str">
@@ -3636,15 +3634,15 @@
       </c>
       <c r="M19" s="95" t="str">
         <f t="shared" si="6"/>
-        <v>obj_0033b#0001</v>
+        <v>obj_00324#0001</v>
       </c>
       <c r="N19" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M19,Trigger),"--")</f>
-        <v>USDFUT3MU6_Quote</v>
+        <v>USDFUT3MZ6_Quote</v>
       </c>
       <c r="O19" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M19,Trigger),"--")</f>
-        <v>99.057500000000005</v>
+        <v>98.887500000000003</v>
       </c>
       <c r="P19" s="98" t="b">
         <v>1</v>
@@ -3657,26 +3655,26 @@
       </c>
       <c r="S19" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M19,Trigger),"--")</f>
-        <v>42634</v>
+        <v>42725</v>
       </c>
       <c r="T19" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M19,Trigger),"--")</f>
-        <v>42725</v>
+        <v>42815</v>
       </c>
       <c r="V19" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Sw</v>
       </c>
       <c r="W19" s="3" t="str">
-        <v>obj_00331</v>
+        <v>obj_00318</v>
       </c>
       <c r="X19" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W19,Trigger),"")</f>
-        <v>USDAM3L6Y_Quote</v>
+        <v>USDAM3L5Y_Quote</v>
       </c>
       <c r="Y19" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W19,Trigger),"")</f>
-        <v>1.7520000000000001E-2</v>
+        <v>1.6490000000000001E-2</v>
       </c>
       <c r="Z19" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W19)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W19)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W19)),_xll.qlSwapRateHelperSpread($W19))</f>
@@ -3684,14 +3682,14 @@
       </c>
       <c r="AA19" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W19,Trigger),"")</f>
-        <v>42257</v>
+        <v>42321</v>
       </c>
       <c r="AB19" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W19,Trigger),"")</f>
-        <v>44449</v>
+        <v>44148</v>
       </c>
       <c r="AC19" s="68">
-        <v>1.7810741266284475E-2</v>
+        <v>1.6708915107592533E-2</v>
       </c>
       <c r="AH19" s="161"/>
     </row>
@@ -3704,7 +3702,7 @@
       </c>
       <c r="C20" s="61" t="str">
         <f>_xll.qlIMMNextCode(C19,B20,Trigger)</f>
-        <v>M6</v>
+        <v>U6</v>
       </c>
       <c r="D20" s="126"/>
       <c r="E20" s="126"/>
@@ -3715,15 +3713,15 @@
       </c>
       <c r="H20" s="120" t="str">
         <f t="shared" si="8"/>
-        <v>USDFUT3MM6_Quote</v>
+        <v>USDFUT3MU6_Quote</v>
       </c>
       <c r="I20" s="120" t="str">
         <f t="shared" si="9"/>
-        <v>USDFUT3MM6ConvAdj_Quote</v>
+        <v>USDFUT3MU6ConvAdj_Quote</v>
       </c>
       <c r="J20" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H20,$H$12,C20,G20,I20,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0033a#0001</v>
+        <v>obj_00323#0001</v>
       </c>
       <c r="K20" s="48"/>
       <c r="L20" s="9" t="str">
@@ -3732,15 +3730,15 @@
       </c>
       <c r="M20" s="95" t="str">
         <f t="shared" si="6"/>
-        <v>obj_0033c#0001</v>
+        <v>obj_00325#0001</v>
       </c>
       <c r="N20" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M20,Trigger),"--")</f>
-        <v>USDFUT3MZ6_Quote</v>
+        <v>USDFUT3MH7_Quote</v>
       </c>
       <c r="O20" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M20,Trigger),"--")</f>
-        <v>98.872500000000002</v>
+        <v>98.727499999999992</v>
       </c>
       <c r="P20" s="98" t="b">
         <v>1</v>
@@ -3753,26 +3751,26 @@
       </c>
       <c r="S20" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M20,Trigger),"--")</f>
-        <v>42725</v>
+        <v>42809</v>
       </c>
       <c r="T20" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M20,Trigger),"--")</f>
-        <v>42815</v>
+        <v>42901</v>
       </c>
       <c r="V20" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Sw</v>
       </c>
       <c r="W20" s="3" t="str">
-        <v>obj_0032a</v>
+        <v>obj_0031c</v>
       </c>
       <c r="X20" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W20,Trigger),"")</f>
-        <v>USDAM3L7Y_Quote</v>
+        <v>USDAM3L6Y_Quote</v>
       </c>
       <c r="Y20" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W20,Trigger),"")</f>
-        <v>1.9009999999999999E-2</v>
+        <v>1.805E-2</v>
       </c>
       <c r="Z20" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W20)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W20)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W20)),_xll.qlSwapRateHelperSpread($W20))</f>
@@ -3780,14 +3778,14 @@
       </c>
       <c r="AA20" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W20,Trigger),"")</f>
-        <v>42257</v>
+        <v>42321</v>
       </c>
       <c r="AB20" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W20,Trigger),"")</f>
-        <v>44816</v>
+        <v>44515</v>
       </c>
       <c r="AC20" s="68">
-        <v>1.937042697999472E-2</v>
+        <v>1.8325703145799729E-2</v>
       </c>
       <c r="AH20" s="161"/>
     </row>
@@ -3800,7 +3798,7 @@
       </c>
       <c r="C21" s="61" t="str">
         <f>_xll.qlIMMNextCode(C20,B21,Trigger)</f>
-        <v>U6</v>
+        <v>Z6</v>
       </c>
       <c r="D21" s="126"/>
       <c r="E21" s="126"/>
@@ -3811,15 +3809,15 @@
       </c>
       <c r="H21" s="120" t="str">
         <f t="shared" si="8"/>
-        <v>USDFUT3MU6_Quote</v>
+        <v>USDFUT3MZ6_Quote</v>
       </c>
       <c r="I21" s="120" t="str">
         <f t="shared" si="9"/>
-        <v>USDFUT3MU6ConvAdj_Quote</v>
+        <v>USDFUT3MZ6ConvAdj_Quote</v>
       </c>
       <c r="J21" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H21,$H$12,C21,G21,I21,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0033b#0001</v>
+        <v>obj_00324#0001</v>
       </c>
       <c r="K21" s="48"/>
       <c r="L21" s="9" t="str">
@@ -3828,15 +3826,15 @@
       </c>
       <c r="M21" s="95" t="str">
         <f t="shared" si="6"/>
-        <v>obj_0033d#0001</v>
+        <v>obj_00326#0001</v>
       </c>
       <c r="N21" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M21,Trigger),"--")</f>
-        <v>USDFUT3MH7_Quote</v>
+        <v>USDFUT3MM7_Quote</v>
       </c>
       <c r="O21" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M21,Trigger),"--")</f>
-        <v>98.717500000000001</v>
+        <v>98.5625</v>
       </c>
       <c r="P21" s="98" t="b">
         <v>1</v>
@@ -3849,26 +3847,26 @@
       </c>
       <c r="S21" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M21,Trigger),"--")</f>
-        <v>42809</v>
+        <v>42907</v>
       </c>
       <c r="T21" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M21,Trigger),"--")</f>
-        <v>42901</v>
+        <v>42999</v>
       </c>
       <c r="V21" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Sw</v>
       </c>
       <c r="W21" s="3" t="str">
-        <v>obj_00325</v>
+        <v>obj_0030f</v>
       </c>
       <c r="X21" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W21,Trigger),"")</f>
-        <v>USDAM3L8Y_Quote</v>
+        <v>USDAM3L7Y_Quote</v>
       </c>
       <c r="Y21" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W21,Trigger),"")</f>
-        <v>2.0219999999999998E-2</v>
+        <v>1.9340000000000003E-2</v>
       </c>
       <c r="Z21" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W21)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W21)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W21)),_xll.qlSwapRateHelperSpread($W21))</f>
@@ -3876,14 +3874,14 @@
       </c>
       <c r="AA21" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W21,Trigger),"")</f>
-        <v>42257</v>
+        <v>42321</v>
       </c>
       <c r="AB21" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W21,Trigger),"")</f>
-        <v>45180</v>
+        <v>44879</v>
       </c>
       <c r="AC21" s="68">
-        <v>2.0647148764555513E-2</v>
+        <v>1.9673709338582632E-2</v>
       </c>
       <c r="AH21" s="161"/>
     </row>
@@ -3896,7 +3894,7 @@
       </c>
       <c r="C22" s="61" t="str">
         <f>_xll.qlIMMNextCode(C21,B22,Trigger)</f>
-        <v>Z6</v>
+        <v>H7</v>
       </c>
       <c r="D22" s="126"/>
       <c r="E22" s="126"/>
@@ -3907,15 +3905,15 @@
       </c>
       <c r="H22" s="120" t="str">
         <f t="shared" si="8"/>
-        <v>USDFUT3MZ6_Quote</v>
+        <v>USDFUT3MH7_Quote</v>
       </c>
       <c r="I22" s="120" t="str">
         <f t="shared" si="9"/>
-        <v>USDFUT3MZ6ConvAdj_Quote</v>
+        <v>USDFUT3MH7ConvAdj_Quote</v>
       </c>
       <c r="J22" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H22,$H$12,C22,G22,I22,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0033c#0001</v>
+        <v>obj_00325#0001</v>
       </c>
       <c r="K22" s="48"/>
       <c r="L22" s="9" t="str">
@@ -3924,15 +3922,15 @@
       </c>
       <c r="M22" s="95" t="str">
         <f t="shared" si="6"/>
-        <v>obj_0033e#0001</v>
+        <v>obj_00327#0001</v>
       </c>
       <c r="N22" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M22,Trigger),"--")</f>
-        <v>USDFUT3MM7_Quote</v>
+        <v>USDFUT3MU7_Quote</v>
       </c>
       <c r="O22" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M22,Trigger),"--")</f>
-        <v>98.5625</v>
+        <v>98.407499999999999</v>
       </c>
       <c r="P22" s="98" t="b">
         <v>1</v>
@@ -3945,26 +3943,26 @@
       </c>
       <c r="S22" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M22,Trigger),"--")</f>
-        <v>42907</v>
+        <v>42998</v>
       </c>
       <c r="T22" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M22,Trigger),"--")</f>
-        <v>42999</v>
+        <v>43089</v>
       </c>
       <c r="V22" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Sw</v>
       </c>
       <c r="W22" s="3" t="str">
-        <v>obj_0032d</v>
+        <v>obj_00319</v>
       </c>
       <c r="X22" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W22,Trigger),"")</f>
-        <v>USDAM3L9Y_Quote</v>
+        <v>USDAM3L8Y_Quote</v>
       </c>
       <c r="Y22" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W22,Trigger),"")</f>
-        <v>2.121E-2</v>
+        <v>2.0400000000000001E-2</v>
       </c>
       <c r="Z22" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W22)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W22)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W22)),_xll.qlSwapRateHelperSpread($W22))</f>
@@ -3972,14 +3970,14 @@
       </c>
       <c r="AA22" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W22,Trigger),"")</f>
-        <v>42257</v>
+        <v>42321</v>
       </c>
       <c r="AB22" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W22,Trigger),"")</f>
-        <v>45545</v>
+        <v>45243</v>
       </c>
       <c r="AC22" s="68">
-        <v>2.1698763087005649E-2</v>
+        <v>2.0800335661726455E-2</v>
       </c>
       <c r="AH22" s="161"/>
     </row>
@@ -3992,7 +3990,7 @@
       </c>
       <c r="C23" s="61" t="str">
         <f>_xll.qlIMMNextCode(C22,B23,Trigger)</f>
-        <v>H7</v>
+        <v>M7</v>
       </c>
       <c r="D23" s="126"/>
       <c r="E23" s="126"/>
@@ -4003,15 +4001,15 @@
       </c>
       <c r="H23" s="120" t="str">
         <f t="shared" si="8"/>
-        <v>USDFUT3MH7_Quote</v>
+        <v>USDFUT3MM7_Quote</v>
       </c>
       <c r="I23" s="120" t="str">
         <f t="shared" si="9"/>
-        <v>USDFUT3MH7ConvAdj_Quote</v>
+        <v>USDFUT3MM7ConvAdj_Quote</v>
       </c>
       <c r="J23" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H23,$H$12,C23,G23,I23,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0033d#0001</v>
+        <v>obj_00326#0001</v>
       </c>
       <c r="K23" s="48"/>
       <c r="L23" s="9" t="str">
@@ -4020,15 +4018,15 @@
       </c>
       <c r="M23" s="95" t="str">
         <f t="shared" si="6"/>
-        <v>obj_0033f#0001</v>
+        <v>obj_00328#0001</v>
       </c>
       <c r="N23" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M23,Trigger),"--")</f>
-        <v>USDFUT3MU7_Quote</v>
+        <v>USDFUT3MZ7_Quote</v>
       </c>
       <c r="O23" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M23,Trigger),"--")</f>
-        <v>98.427500000000009</v>
+        <v>98.259999999999991</v>
       </c>
       <c r="P23" s="98" t="b">
         <v>1</v>
@@ -4041,26 +4039,26 @@
       </c>
       <c r="S23" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M23,Trigger),"--")</f>
-        <v>42998</v>
+        <v>43089</v>
       </c>
       <c r="T23" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M23,Trigger),"--")</f>
-        <v>43089</v>
+        <v>43179</v>
       </c>
       <c r="V23" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Sw</v>
       </c>
       <c r="W23" s="3" t="str">
-        <v>obj_00330</v>
+        <v>obj_00310</v>
       </c>
       <c r="X23" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W23,Trigger),"")</f>
-        <v>USDAM3L10Y_Quote</v>
+        <v>USDAM3L9Y_Quote</v>
       </c>
       <c r="Y23" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W23,Trigger),"")</f>
-        <v>2.2040000000000001E-2</v>
+        <v>2.128E-2</v>
       </c>
       <c r="Z23" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W23)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W23)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W23)),_xll.qlSwapRateHelperSpread($W23))</f>
@@ -4068,14 +4066,14 @@
       </c>
       <c r="AA23" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W23,Trigger),"")</f>
-        <v>42257</v>
+        <v>42321</v>
       </c>
       <c r="AB23" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W23,Trigger),"")</f>
-        <v>45910</v>
+        <v>45609</v>
       </c>
       <c r="AC23" s="68">
-        <v>2.2586669113882674E-2</v>
+        <v>2.1732711881939291E-2</v>
       </c>
       <c r="AH23" s="161"/>
     </row>
@@ -4088,7 +4086,7 @@
       </c>
       <c r="C24" s="61" t="str">
         <f>_xll.qlIMMNextCode(C23,B24,Trigger)</f>
-        <v>M7</v>
+        <v>U7</v>
       </c>
       <c r="D24" s="126"/>
       <c r="E24" s="126"/>
@@ -4099,15 +4097,15 @@
       </c>
       <c r="H24" s="120" t="str">
         <f t="shared" si="8"/>
-        <v>USDFUT3MM7_Quote</v>
+        <v>USDFUT3MU7_Quote</v>
       </c>
       <c r="I24" s="120" t="str">
         <f t="shared" si="9"/>
-        <v>USDFUT3MM7ConvAdj_Quote</v>
+        <v>USDFUT3MU7ConvAdj_Quote</v>
       </c>
       <c r="J24" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H24,$H$12,C24,G24,I24,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0033e#0001</v>
+        <v>obj_00327#0001</v>
       </c>
       <c r="K24" s="48"/>
       <c r="L24" s="9" t="str">
@@ -4116,15 +4114,15 @@
       </c>
       <c r="M24" s="95" t="str">
         <f t="shared" si="6"/>
-        <v>obj_00340#0001</v>
+        <v>obj_00329#0001</v>
       </c>
       <c r="N24" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M24,Trigger),"--")</f>
-        <v>USDFUT3MZ7_Quote</v>
+        <v>USDFUT3MH8_Quote</v>
       </c>
       <c r="O24" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M24,Trigger),"--")</f>
-        <v>98.287499999999994</v>
+        <v>98.142499999999998</v>
       </c>
       <c r="P24" s="98" t="b">
         <v>1</v>
@@ -4137,26 +4135,26 @@
       </c>
       <c r="S24" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M24,Trigger),"--")</f>
-        <v>43089</v>
+        <v>43180</v>
       </c>
       <c r="T24" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M24,Trigger),"--")</f>
-        <v>43179</v>
+        <v>43272</v>
       </c>
       <c r="V24" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Sw</v>
       </c>
       <c r="W24" s="3" t="str">
-        <v>obj_00327</v>
+        <v>obj_00314</v>
       </c>
       <c r="X24" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W24,Trigger),"")</f>
-        <v>USDAM3L12Y_Quote</v>
+        <v>USDAM3L10Y_Quote</v>
       </c>
       <c r="Y24" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W24,Trigger),"")</f>
-        <v>2.3359999999999999E-2</v>
+        <v>2.2029999999999998E-2</v>
       </c>
       <c r="Z24" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W24)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W24)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W24)),_xll.qlSwapRateHelperSpread($W24))</f>
@@ -4164,14 +4162,14 @@
       </c>
       <c r="AA24" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W24,Trigger),"")</f>
-        <v>42257</v>
+        <v>42321</v>
       </c>
       <c r="AB24" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W24,Trigger),"")</f>
-        <v>46640</v>
+        <v>45974</v>
       </c>
       <c r="AC24" s="68">
-        <v>2.4014841599207099E-2</v>
+        <v>2.2533521489388968E-2</v>
       </c>
       <c r="AH24" s="161"/>
     </row>
@@ -4184,7 +4182,7 @@
       </c>
       <c r="C25" s="61" t="str">
         <f>_xll.qlIMMNextCode(C24,B25,Trigger)</f>
-        <v>U7</v>
+        <v>Z7</v>
       </c>
       <c r="D25" s="126"/>
       <c r="E25" s="126"/>
@@ -4195,15 +4193,15 @@
       </c>
       <c r="H25" s="120" t="str">
         <f t="shared" si="8"/>
-        <v>USDFUT3MU7_Quote</v>
+        <v>USDFUT3MZ7_Quote</v>
       </c>
       <c r="I25" s="120" t="str">
         <f t="shared" si="9"/>
-        <v>USDFUT3MU7ConvAdj_Quote</v>
+        <v>USDFUT3MZ7ConvAdj_Quote</v>
       </c>
       <c r="J25" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H25,$H$12,C25,G25,I25,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0033f#0001</v>
+        <v>obj_00328#0001</v>
       </c>
       <c r="K25" s="48"/>
       <c r="L25" s="9" t="str">
@@ -4212,15 +4210,15 @@
       </c>
       <c r="M25" s="95" t="str">
         <f t="shared" si="6"/>
-        <v>obj_00341#0001</v>
+        <v>obj_0032a#0001</v>
       </c>
       <c r="N25" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M25,Trigger),"--")</f>
-        <v>USDFUT3MH8_Quote</v>
+        <v>USDFUT3MM8_Quote</v>
       </c>
       <c r="O25" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M25,Trigger),"--")</f>
-        <v>98.172499999999999</v>
+        <v>98.03</v>
       </c>
       <c r="P25" s="98" t="b">
         <v>1</v>
@@ -4233,26 +4231,26 @@
       </c>
       <c r="S25" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M25,Trigger),"--")</f>
-        <v>43180</v>
+        <v>43271</v>
       </c>
       <c r="T25" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M25,Trigger),"--")</f>
-        <v>43272</v>
+        <v>43363</v>
       </c>
       <c r="V25" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Sw</v>
       </c>
       <c r="W25" s="3" t="str">
-        <v>obj_00324</v>
+        <v>obj_00317</v>
       </c>
       <c r="X25" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W25,Trigger),"")</f>
-        <v>USDAM3L15Y_Quote</v>
+        <v>USDAM3L12Y_Quote</v>
       </c>
       <c r="Y25" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W25,Trigger),"")</f>
-        <v>2.4680000000000001E-2</v>
+        <v>2.3279999999999999E-2</v>
       </c>
       <c r="Z25" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W25)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W25)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W25)),_xll.qlSwapRateHelperSpread($W25))</f>
@@ -4260,14 +4258,14 @@
       </c>
       <c r="AA25" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W25,Trigger),"")</f>
-        <v>42257</v>
+        <v>42321</v>
       </c>
       <c r="AB25" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W25,Trigger),"")</f>
-        <v>47736</v>
+        <v>46706</v>
       </c>
       <c r="AC25" s="68">
-        <v>2.5460255809551698E-2</v>
+        <v>2.3886273671146901E-2</v>
       </c>
       <c r="AH25" s="161"/>
     </row>
@@ -4280,7 +4278,7 @@
       </c>
       <c r="C26" s="61" t="str">
         <f>_xll.qlIMMNextCode(C25,B26,Trigger)</f>
-        <v>Z7</v>
+        <v>H8</v>
       </c>
       <c r="D26" s="126"/>
       <c r="E26" s="126"/>
@@ -4291,15 +4289,15 @@
       </c>
       <c r="H26" s="120" t="str">
         <f t="shared" si="8"/>
-        <v>USDFUT3MZ7_Quote</v>
+        <v>USDFUT3MH8_Quote</v>
       </c>
       <c r="I26" s="120" t="str">
         <f t="shared" si="9"/>
-        <v>USDFUT3MZ7ConvAdj_Quote</v>
+        <v>USDFUT3MH8ConvAdj_Quote</v>
       </c>
       <c r="J26" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H26,$H$12,C26,G26,I26,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00340#0001</v>
+        <v>obj_00329#0001</v>
       </c>
       <c r="K26" s="48"/>
       <c r="L26" s="9" t="str">
@@ -4308,15 +4306,15 @@
       </c>
       <c r="M26" s="95" t="str">
         <f t="shared" si="6"/>
-        <v>obj_00342#0001</v>
+        <v>obj_0032b#0001</v>
       </c>
       <c r="N26" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M26,Trigger),"--")</f>
-        <v>USDFUT3MM8_Quote</v>
+        <v>USDFUT3MU8_Quote</v>
       </c>
       <c r="O26" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M26,Trigger),"--")</f>
-        <v>98.057500000000005</v>
+        <v>97.932500000000005</v>
       </c>
       <c r="P26" s="98" t="b">
         <v>1</v>
@@ -4329,26 +4327,26 @@
       </c>
       <c r="S26" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M26,Trigger),"--")</f>
-        <v>43271</v>
+        <v>43362</v>
       </c>
       <c r="T26" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M26,Trigger),"--")</f>
-        <v>43363</v>
+        <v>43453</v>
       </c>
       <c r="V26" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Sw</v>
       </c>
       <c r="W26" s="3" t="str">
-        <v>obj_00332</v>
+        <v>obj_00316</v>
       </c>
       <c r="X26" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W26,Trigger),"")</f>
-        <v>USDAM3L20Y_Quote</v>
+        <v>USDAM3L15Y_Quote</v>
       </c>
       <c r="Y26" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W26,Trigger),"")</f>
-        <v>2.588E-2</v>
+        <v>2.452E-2</v>
       </c>
       <c r="Z26" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W26)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W26)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W26)),_xll.qlSwapRateHelperSpread($W26))</f>
@@ -4356,14 +4354,14 @@
       </c>
       <c r="AA26" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W26,Trigger),"")</f>
-        <v>42257</v>
+        <v>42321</v>
       </c>
       <c r="AB26" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W26,Trigger),"")</f>
-        <v>49562</v>
+        <v>47800</v>
       </c>
       <c r="AC26" s="68">
-        <v>2.6781862613277998E-2</v>
+        <v>2.524412859147766E-2</v>
       </c>
       <c r="AH26" s="161"/>
     </row>
@@ -4376,7 +4374,7 @@
       </c>
       <c r="C27" s="61" t="str">
         <f>_xll.qlIMMNextCode(C26,B27,Trigger)</f>
-        <v>H8</v>
+        <v>M8</v>
       </c>
       <c r="D27" s="126"/>
       <c r="E27" s="126"/>
@@ -4387,15 +4385,15 @@
       </c>
       <c r="H27" s="120" t="str">
         <f t="shared" si="8"/>
-        <v>USDFUT3MH8_Quote</v>
+        <v>USDFUT3MM8_Quote</v>
       </c>
       <c r="I27" s="120" t="str">
         <f t="shared" si="9"/>
-        <v>USDFUT3MH8ConvAdj_Quote</v>
+        <v>USDFUT3MM8ConvAdj_Quote</v>
       </c>
       <c r="J27" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H27,$H$12,C27,G27,I27,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00341#0001</v>
+        <v>obj_0032a#0001</v>
       </c>
       <c r="K27" s="48"/>
       <c r="L27" s="9" t="str">
@@ -4404,15 +4402,15 @@
       </c>
       <c r="M27" s="95" t="str">
         <f t="shared" si="6"/>
-        <v>obj_00343#0001</v>
+        <v>obj_0032c#0001</v>
       </c>
       <c r="N27" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M27,Trigger),"--")</f>
-        <v>USDFUT3MU8_Quote</v>
+        <v>USDFUT3MZ8_Quote</v>
       </c>
       <c r="O27" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M27,Trigger),"--")</f>
-        <v>97.952500000000001</v>
+        <v>97.837500000000006</v>
       </c>
       <c r="P27" s="98" t="b">
         <v>1</v>
@@ -4425,26 +4423,26 @@
       </c>
       <c r="S27" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M27,Trigger),"--")</f>
-        <v>43362</v>
+        <v>43453</v>
       </c>
       <c r="T27" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M27,Trigger),"--")</f>
-        <v>43453</v>
+        <v>43543</v>
       </c>
       <c r="V27" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Sw</v>
       </c>
       <c r="W27" s="3" t="str">
-        <v>obj_0032e</v>
+        <v>obj_00311</v>
       </c>
       <c r="X27" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W27,Trigger),"")</f>
-        <v>USDAM3L25Y_Quote</v>
+        <v>USDAM3L20Y_Quote</v>
       </c>
       <c r="Y27" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W27,Trigger),"")</f>
-        <v>2.6469999999999997E-2</v>
+        <v>2.5770000000000001E-2</v>
       </c>
       <c r="Z27" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W27)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W27)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W27)),_xll.qlSwapRateHelperSpread($W27))</f>
@@ -4452,14 +4450,14 @@
       </c>
       <c r="AA27" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W27,Trigger),"")</f>
-        <v>42257</v>
+        <v>42321</v>
       </c>
       <c r="AB27" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W27,Trigger),"")</f>
-        <v>51389</v>
+        <v>49626</v>
       </c>
       <c r="AC27" s="68">
-        <v>2.7411615288364333E-2</v>
+        <v>2.664067938956842E-2</v>
       </c>
       <c r="AH27" s="161"/>
     </row>
@@ -4472,7 +4470,7 @@
       </c>
       <c r="C28" s="61" t="str">
         <f>_xll.qlIMMNextCode(C27,B28,Trigger)</f>
-        <v>M8</v>
+        <v>U8</v>
       </c>
       <c r="D28" s="126"/>
       <c r="E28" s="126"/>
@@ -4483,15 +4481,15 @@
       </c>
       <c r="H28" s="120" t="str">
         <f t="shared" si="8"/>
-        <v>USDFUT3MM8_Quote</v>
+        <v>USDFUT3MU8_Quote</v>
       </c>
       <c r="I28" s="120" t="str">
         <f t="shared" si="9"/>
-        <v>USDFUT3MM8ConvAdj_Quote</v>
+        <v>USDFUT3MU8ConvAdj_Quote</v>
       </c>
       <c r="J28" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H28,$H$12,C28,G28,I28,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00342#0001</v>
+        <v>obj_0032b#0001</v>
       </c>
       <c r="K28" s="48"/>
       <c r="L28" s="9" t="str">
@@ -4500,15 +4498,15 @@
       </c>
       <c r="M28" s="95" t="str">
         <f t="shared" si="6"/>
-        <v>obj_00344#0001</v>
+        <v>obj_0032d#0001</v>
       </c>
       <c r="N28" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M28,Trigger),"--")</f>
-        <v>USDFUT3MZ8_Quote</v>
+        <v>USDFUT3MH9_Quote</v>
       </c>
       <c r="O28" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M28,Trigger),"--")</f>
-        <v>97.847499999999997</v>
+        <v>97.759999999999991</v>
       </c>
       <c r="P28" s="98" t="b">
         <v>1</v>
@@ -4521,26 +4519,26 @@
       </c>
       <c r="S28" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M28,Trigger),"--")</f>
-        <v>43453</v>
+        <v>43544</v>
       </c>
       <c r="T28" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M28,Trigger),"--")</f>
-        <v>43543</v>
+        <v>43636</v>
       </c>
       <c r="V28" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Sw</v>
       </c>
       <c r="W28" s="3" t="str">
-        <v>obj_0032f</v>
+        <v>obj_00313</v>
       </c>
       <c r="X28" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W28,Trigger),"")</f>
-        <v>USDAM3L30Y_Quote</v>
+        <v>USDAM3L25Y_Quote</v>
       </c>
       <c r="Y28" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W28,Trigger),"")</f>
-        <v>2.6830000000000003E-2</v>
+        <v>2.6309999999999997E-2</v>
       </c>
       <c r="Z28" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W28)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W28)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W28)),_xll.qlSwapRateHelperSpread($W28))</f>
@@ -4548,14 +4546,14 @@
       </c>
       <c r="AA28" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W28,Trigger),"")</f>
-        <v>42257</v>
+        <v>42321</v>
       </c>
       <c r="AB28" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W28,Trigger),"")</f>
-        <v>53216</v>
+        <v>51453</v>
       </c>
       <c r="AC28" s="68">
-        <v>2.7791519255449992E-2</v>
+        <v>2.7194336839467616E-2</v>
       </c>
       <c r="AH28" s="161"/>
     </row>
@@ -4568,7 +4566,7 @@
       </c>
       <c r="C29" s="61" t="str">
         <f>_xll.qlIMMNextCode(C28,B29,Trigger)</f>
-        <v>U8</v>
+        <v>Z8</v>
       </c>
       <c r="D29" s="126"/>
       <c r="E29" s="126"/>
@@ -4579,15 +4577,15 @@
       </c>
       <c r="H29" s="120" t="str">
         <f t="shared" si="8"/>
-        <v>USDFUT3MU8_Quote</v>
+        <v>USDFUT3MZ8_Quote</v>
       </c>
       <c r="I29" s="120" t="str">
         <f t="shared" si="9"/>
-        <v>USDFUT3MU8ConvAdj_Quote</v>
+        <v>USDFUT3MZ8ConvAdj_Quote</v>
       </c>
       <c r="J29" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H29,$H$12,C29,G29,I29,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00343#0001</v>
+        <v>obj_0032c#0001</v>
       </c>
       <c r="K29" s="48"/>
       <c r="L29" s="9" t="str">
@@ -4596,15 +4594,15 @@
       </c>
       <c r="M29" s="95" t="str">
         <f t="shared" si="6"/>
-        <v>obj_00345#0001</v>
+        <v>obj_0032e#0001</v>
       </c>
       <c r="N29" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M29,Trigger),"--")</f>
-        <v>USDFUT3MH9_Quote</v>
+        <v>USDFUT3MM9_Quote</v>
       </c>
       <c r="O29" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M29,Trigger),"--")</f>
-        <v>97.759999999999991</v>
+        <v>97.682500000000005</v>
       </c>
       <c r="P29" s="98" t="b">
         <v>1</v>
@@ -4617,41 +4615,41 @@
       </c>
       <c r="S29" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M29,Trigger),"--")</f>
-        <v>43544</v>
+        <v>43635</v>
       </c>
       <c r="T29" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M29,Trigger),"--")</f>
-        <v>43636</v>
+        <v>43727</v>
       </c>
       <c r="V29" s="3" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="W29" s="3" t="e">
-        <v>#N/A</v>
+        <v>Sw</v>
+      </c>
+      <c r="W29" s="3" t="str">
+        <v>obj_0031b</v>
       </c>
       <c r="X29" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W29,Trigger),"")</f>
-        <v/>
-      </c>
-      <c r="Y29" s="68" t="str">
+        <v>USDAM3L30Y_Quote</v>
+      </c>
+      <c r="Y29" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W29,Trigger),"")</f>
-        <v/>
-      </c>
-      <c r="Z29" s="105" t="str">
+        <v>2.6619999999999998E-2</v>
+      </c>
+      <c r="Z29" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W29)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W29)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W29)),_xll.qlSwapRateHelperSpread($W29))</f>
-        <v/>
-      </c>
-      <c r="AA29" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="AA29" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W29,Trigger),"")</f>
-        <v/>
-      </c>
-      <c r="AB29" s="4" t="str">
+        <v>42321</v>
+      </c>
+      <c r="AB29" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W29,Trigger),"")</f>
-        <v/>
-      </c>
-      <c r="AC29" s="68" t="e">
-        <v>#N/A</v>
+        <v>53279</v>
+      </c>
+      <c r="AC29" s="68">
+        <v>2.7507350218453085E-2</v>
       </c>
       <c r="AH29" s="161"/>
     </row>
@@ -4664,7 +4662,7 @@
       </c>
       <c r="C30" s="61" t="str">
         <f>_xll.qlIMMNextCode(C29,B30,Trigger)</f>
-        <v>Z8</v>
+        <v>H9</v>
       </c>
       <c r="D30" s="126"/>
       <c r="E30" s="126"/>
@@ -4675,15 +4673,15 @@
       </c>
       <c r="H30" s="120" t="str">
         <f t="shared" si="8"/>
-        <v>USDFUT3MZ8_Quote</v>
+        <v>USDFUT3MH9_Quote</v>
       </c>
       <c r="I30" s="120" t="str">
         <f t="shared" si="9"/>
-        <v>USDFUT3MZ8ConvAdj_Quote</v>
+        <v>USDFUT3MH9ConvAdj_Quote</v>
       </c>
       <c r="J30" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H30,$H$12,C30,G30,I30,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00344#0001</v>
+        <v>obj_0032d#0001</v>
       </c>
       <c r="K30" s="48"/>
       <c r="L30" s="9" t="str">
@@ -4692,15 +4690,15 @@
       </c>
       <c r="M30" s="95" t="str">
         <f t="shared" si="6"/>
-        <v>obj_00346#0001</v>
+        <v>obj_0032f#0001</v>
       </c>
       <c r="N30" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M30,Trigger),"--")</f>
-        <v>USDFUT3MM9_Quote</v>
+        <v>USDFUT3MU9_Quote</v>
       </c>
       <c r="O30" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M30,Trigger),"--")</f>
-        <v>97.667500000000004</v>
+        <v>97.61</v>
       </c>
       <c r="P30" s="98" t="b">
         <v>1</v>
@@ -4713,41 +4711,41 @@
       </c>
       <c r="S30" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M30,Trigger),"--")</f>
-        <v>43635</v>
+        <v>43726</v>
       </c>
       <c r="T30" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M30,Trigger),"--")</f>
-        <v>43727</v>
+        <v>43817</v>
       </c>
       <c r="V30" s="3" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="W30" s="3" t="e">
-        <v>#N/A</v>
+        <v>Sw</v>
+      </c>
+      <c r="W30" s="3" t="str">
+        <v>obj_00312</v>
       </c>
       <c r="X30" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W30,Trigger),"")</f>
-        <v/>
-      </c>
-      <c r="Y30" s="68" t="str">
+        <v>USDAM3L40Y_Quote</v>
+      </c>
+      <c r="Y30" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W30,Trigger),"")</f>
-        <v/>
-      </c>
-      <c r="Z30" s="105" t="str">
+        <v>2.6789999999999998E-2</v>
+      </c>
+      <c r="Z30" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W30)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W30)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W30)),_xll.qlSwapRateHelperSpread($W30))</f>
-        <v/>
-      </c>
-      <c r="AA30" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="AA30" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W30,Trigger),"")</f>
-        <v/>
-      </c>
-      <c r="AB30" s="4" t="str">
+        <v>42321</v>
+      </c>
+      <c r="AB30" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W30,Trigger),"")</f>
-        <v/>
-      </c>
-      <c r="AC30" s="68" t="e">
-        <v>#N/A</v>
+        <v>56933</v>
+      </c>
+      <c r="AC30" s="68">
+        <v>2.7578731092807302E-2</v>
       </c>
       <c r="AH30" s="161"/>
     </row>
@@ -4760,7 +4758,7 @@
       </c>
       <c r="C31" s="61" t="str">
         <f>_xll.qlIMMNextCode(C30,B31,Trigger)</f>
-        <v>H9</v>
+        <v>M9</v>
       </c>
       <c r="D31" s="126"/>
       <c r="E31" s="126"/>
@@ -4771,15 +4769,15 @@
       </c>
       <c r="H31" s="120" t="str">
         <f t="shared" si="8"/>
-        <v>USDFUT3MH9_Quote</v>
+        <v>USDFUT3MM9_Quote</v>
       </c>
       <c r="I31" s="120" t="str">
         <f t="shared" si="9"/>
-        <v>USDFUT3MH9ConvAdj_Quote</v>
+        <v>USDFUT3MM9ConvAdj_Quote</v>
       </c>
       <c r="J31" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H31,$H$12,C31,G31,I31,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00345#0001</v>
+        <v>obj_0032e#0001</v>
       </c>
       <c r="K31" s="48"/>
       <c r="L31" s="9" t="str">
@@ -4788,15 +4786,15 @@
       </c>
       <c r="M31" s="95" t="str">
         <f t="shared" si="6"/>
-        <v>obj_00347#0001</v>
+        <v>obj_00330#0001</v>
       </c>
       <c r="N31" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M31,Trigger),"--")</f>
-        <v>USDFUT3MU9_Quote</v>
+        <v>USDFUT3MZ9_Quote</v>
       </c>
       <c r="O31" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M31,Trigger),"--")</f>
-        <v>97.582499999999996</v>
+        <v>97.537499999999994</v>
       </c>
       <c r="P31" s="98" t="b">
         <v>1</v>
@@ -4809,41 +4807,41 @@
       </c>
       <c r="S31" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M31,Trigger),"--")</f>
-        <v>43726</v>
+        <v>43817</v>
       </c>
       <c r="T31" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M31,Trigger),"--")</f>
-        <v>43817</v>
+        <v>43908</v>
       </c>
       <c r="V31" s="3" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="W31" s="3" t="e">
-        <v>#N/A</v>
+        <v>Sw</v>
+      </c>
+      <c r="W31" s="3" t="str">
+        <v>obj_0031a</v>
       </c>
       <c r="X31" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W31,Trigger),"")</f>
-        <v/>
-      </c>
-      <c r="Y31" s="68" t="str">
+        <v>USDAM3L50Y_Quote</v>
+      </c>
+      <c r="Y31" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W31,Trigger),"")</f>
-        <v/>
-      </c>
-      <c r="Z31" s="105" t="str">
+        <v>2.6670000000000003E-2</v>
+      </c>
+      <c r="Z31" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W31)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W31)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W31)),_xll.qlSwapRateHelperSpread($W31))</f>
-        <v/>
-      </c>
-      <c r="AA31" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="AA31" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W31,Trigger),"")</f>
-        <v/>
-      </c>
-      <c r="AB31" s="4" t="str">
+        <v>42321</v>
+      </c>
+      <c r="AB31" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W31,Trigger),"")</f>
-        <v/>
-      </c>
-      <c r="AC31" s="68" t="e">
-        <v>#N/A</v>
+        <v>60584</v>
+      </c>
+      <c r="AC31" s="68">
+        <v>2.7177161234110167E-2</v>
       </c>
       <c r="AH31" s="161"/>
     </row>
@@ -4856,7 +4854,7 @@
       </c>
       <c r="C32" s="61" t="str">
         <f>_xll.qlIMMNextCode(C31,B32,Trigger)</f>
-        <v>M9</v>
+        <v>U9</v>
       </c>
       <c r="D32" s="126"/>
       <c r="E32" s="126"/>
@@ -4867,15 +4865,15 @@
       </c>
       <c r="H32" s="120" t="str">
         <f t="shared" si="8"/>
-        <v>USDFUT3MM9_Quote</v>
+        <v>USDFUT3MU9_Quote</v>
       </c>
       <c r="I32" s="120" t="str">
         <f t="shared" si="9"/>
-        <v>USDFUT3MM9ConvAdj_Quote</v>
+        <v>USDFUT3MU9ConvAdj_Quote</v>
       </c>
       <c r="J32" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H32,$H$12,C32,G32,I32,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00346#0001</v>
+        <v>obj_0032f#0001</v>
       </c>
       <c r="K32" s="48"/>
       <c r="L32" s="9" t="str">
@@ -4884,15 +4882,15 @@
       </c>
       <c r="M32" s="95" t="str">
         <f t="shared" si="6"/>
-        <v>obj_00348#0001</v>
+        <v>obj_00331#0001</v>
       </c>
       <c r="N32" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M32,Trigger),"--")</f>
-        <v>USDFUT3MZ9_Quote</v>
+        <v>USDFUT3MH0_Quote</v>
       </c>
       <c r="O32" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M32,Trigger),"--")</f>
-        <v>97.497500000000002</v>
+        <v>97.472499999999997</v>
       </c>
       <c r="P32" s="98" t="b">
         <v>1</v>
@@ -4905,11 +4903,11 @@
       </c>
       <c r="S32" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M32,Trigger),"--")</f>
-        <v>43817</v>
+        <v>43908</v>
       </c>
       <c r="T32" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M32,Trigger),"--")</f>
-        <v>43908</v>
+        <v>44000</v>
       </c>
       <c r="V32" s="3" t="str">
         <f t="shared" si="1"/>
@@ -4951,7 +4949,7 @@
       </c>
       <c r="C33" s="61" t="str">
         <f>_xll.qlIMMNextCode(C32,B33,Trigger)</f>
-        <v>U9</v>
+        <v>Z9</v>
       </c>
       <c r="D33" s="126"/>
       <c r="E33" s="126"/>
@@ -4962,15 +4960,15 @@
       </c>
       <c r="H33" s="120" t="str">
         <f t="shared" si="8"/>
-        <v>USDFUT3MU9_Quote</v>
+        <v>USDFUT3MZ9_Quote</v>
       </c>
       <c r="I33" s="120" t="str">
         <f t="shared" si="9"/>
-        <v>USDFUT3MU9ConvAdj_Quote</v>
+        <v>USDFUT3MZ9ConvAdj_Quote</v>
       </c>
       <c r="J33" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H33,$H$12,C33,G33,I33,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00347#0001</v>
+        <v>obj_00330#0001</v>
       </c>
       <c r="K33" s="48"/>
       <c r="L33" s="10" t="str">
@@ -4979,15 +4977,15 @@
       </c>
       <c r="M33" s="96" t="str">
         <f t="shared" si="6"/>
-        <v>obj_00349#0001</v>
+        <v>obj_00332#0001</v>
       </c>
       <c r="N33" s="149" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M33,Trigger),"--")</f>
-        <v>USDFUT3MH0_Quote</v>
+        <v>USDFUT3MM0_Quote</v>
       </c>
       <c r="O33" s="154">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M33,Trigger),"--")</f>
-        <v>97.417500000000004</v>
+        <v>97.407499999999999</v>
       </c>
       <c r="P33" s="101" t="b">
         <v>1</v>
@@ -5000,11 +4998,11 @@
       </c>
       <c r="S33" s="103">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M33,Trigger),"--")</f>
-        <v>43908</v>
+        <v>43999</v>
       </c>
       <c r="T33" s="103">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M33,Trigger),"--")</f>
-        <v>44000</v>
+        <v>44091</v>
       </c>
       <c r="V33" s="3" t="str">
         <f t="shared" si="1"/>
@@ -5046,7 +5044,7 @@
       </c>
       <c r="C34" s="61" t="str">
         <f>_xll.qlIMMNextCode(C33,B34,Trigger)</f>
-        <v>Z9</v>
+        <v>H0</v>
       </c>
       <c r="D34" s="126"/>
       <c r="E34" s="126"/>
@@ -5057,15 +5055,15 @@
       </c>
       <c r="H34" s="120" t="str">
         <f t="shared" si="8"/>
-        <v>USDFUT3MZ9_Quote</v>
+        <v>USDFUT3MH0_Quote</v>
       </c>
       <c r="I34" s="120" t="str">
         <f t="shared" si="9"/>
-        <v>USDFUT3MZ9ConvAdj_Quote</v>
+        <v>USDFUT3MH0ConvAdj_Quote</v>
       </c>
       <c r="J34" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H34,$H$12,C34,G34,I34,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00348#0001</v>
+        <v>obj_00331#0001</v>
       </c>
       <c r="K34" s="48"/>
       <c r="L34" s="137" t="str">
@@ -5141,7 +5139,7 @@
       </c>
       <c r="C35" s="8" t="str">
         <f>_xll.qlIMMNextCode(C34,B35,Trigger)</f>
-        <v>H0</v>
+        <v>M0</v>
       </c>
       <c r="D35" s="127"/>
       <c r="E35" s="127"/>
@@ -5152,15 +5150,15 @@
       </c>
       <c r="H35" s="121" t="str">
         <f t="shared" si="8"/>
-        <v>USDFUT3MH0_Quote</v>
+        <v>USDFUT3MM0_Quote</v>
       </c>
       <c r="I35" s="121" t="str">
         <f t="shared" si="9"/>
-        <v>USDFUT3MH0ConvAdj_Quote</v>
+        <v>USDFUT3MM0ConvAdj_Quote</v>
       </c>
       <c r="J35" s="2" t="str">
         <f>_xll.qlFuturesRateHelper(,H35,$H$12,C35,G35,I35,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00349#0001</v>
+        <v>obj_00332#0001</v>
       </c>
       <c r="K35" s="48"/>
       <c r="L35" s="69" t="str">
@@ -5433,7 +5431,7 @@
       </c>
       <c r="M38" s="142" t="str">
         <f t="shared" si="11"/>
-        <v>obj_00319#0001</v>
+        <v>obj_00301#0001</v>
       </c>
       <c r="N38" s="151" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M38,Trigger),"--")</f>
@@ -5441,7 +5439,7 @@
       </c>
       <c r="O38" s="144">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M38,Trigger),"--")</f>
-        <v>8.5599999999999999E-3</v>
+        <v>9.4699999999999993E-3</v>
       </c>
       <c r="P38" s="143" t="b">
         <v>1</v>
@@ -5454,11 +5452,11 @@
       </c>
       <c r="S38" s="145">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M38,Trigger),"--")</f>
-        <v>42257</v>
+        <v>42321</v>
       </c>
       <c r="T38" s="145">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M38,Trigger),"--")</f>
-        <v>42989</v>
+        <v>43052</v>
       </c>
       <c r="V38" s="3" t="str">
         <f t="shared" si="12"/>
@@ -5529,7 +5527,7 @@
       </c>
       <c r="M39" s="142" t="str">
         <f t="shared" si="11"/>
-        <v>obj_0032c#0001</v>
+        <v>obj_0030e#0001</v>
       </c>
       <c r="N39" s="151" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M39,Trigger),"--")</f>
@@ -5537,7 +5535,7 @@
       </c>
       <c r="O39" s="144">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M39,Trigger),"--")</f>
-        <v>1.1339999999999999E-2</v>
+        <v>1.2359999999999999E-2</v>
       </c>
       <c r="P39" s="143" t="b">
         <v>1</v>
@@ -5550,11 +5548,11 @@
       </c>
       <c r="S39" s="145">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M39,Trigger),"--")</f>
-        <v>42257</v>
+        <v>42321</v>
       </c>
       <c r="T39" s="145">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M39,Trigger),"--")</f>
-        <v>43353</v>
+        <v>43417</v>
       </c>
       <c r="V39" s="3" t="str">
         <f t="shared" si="12"/>
@@ -5625,7 +5623,7 @@
       </c>
       <c r="M40" s="142" t="str">
         <f t="shared" si="11"/>
-        <v>obj_00329#0001</v>
+        <v>obj_0030d#0001</v>
       </c>
       <c r="N40" s="151" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M40,Trigger),"--")</f>
@@ -5633,7 +5631,7 @@
       </c>
       <c r="O40" s="144">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M40,Trigger),"--")</f>
-        <v>1.3729999999999999E-2</v>
+        <v>1.4649999999999998E-2</v>
       </c>
       <c r="P40" s="143" t="b">
         <v>1</v>
@@ -5646,11 +5644,11 @@
       </c>
       <c r="S40" s="145">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M40,Trigger),"--")</f>
-        <v>42257</v>
+        <v>42321</v>
       </c>
       <c r="T40" s="145">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M40,Trigger),"--")</f>
-        <v>43718</v>
+        <v>43782</v>
       </c>
       <c r="V40" s="3" t="str">
         <f t="shared" si="12"/>
@@ -5720,7 +5718,7 @@
       </c>
       <c r="M41" s="142" t="str">
         <f t="shared" si="11"/>
-        <v>obj_0032b#0001</v>
+        <v>obj_00318#0001</v>
       </c>
       <c r="N41" s="151" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M41,Trigger),"--")</f>
@@ -5728,7 +5726,7 @@
       </c>
       <c r="O41" s="144">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M41,Trigger),"--")</f>
-        <v>1.5769999999999999E-2</v>
+        <v>1.6490000000000001E-2</v>
       </c>
       <c r="P41" s="143" t="b">
         <v>1</v>
@@ -5741,11 +5739,11 @@
       </c>
       <c r="S41" s="145">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M41,Trigger),"--")</f>
-        <v>42257</v>
+        <v>42321</v>
       </c>
       <c r="T41" s="145">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M41,Trigger),"--")</f>
-        <v>44084</v>
+        <v>44148</v>
       </c>
       <c r="V41" s="3" t="str">
         <f t="shared" si="12"/>
@@ -5810,7 +5808,7 @@
       </c>
       <c r="J42" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H42,,B42,JoinCalendar,USDSTD!D42,USDSTD!E42,USDSTD!F42,USDSTD!G42,USDSTD!I42,USDSTD!C42,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00319#0001</v>
+        <v>obj_00301#0001</v>
       </c>
       <c r="L42" s="69" t="str">
         <f t="shared" si="10"/>
@@ -5818,7 +5816,7 @@
       </c>
       <c r="M42" s="142" t="str">
         <f t="shared" si="11"/>
-        <v>obj_00331#0001</v>
+        <v>obj_0031c#0001</v>
       </c>
       <c r="N42" s="151" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M42,Trigger),"--")</f>
@@ -5826,7 +5824,7 @@
       </c>
       <c r="O42" s="144">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M42,Trigger),"--")</f>
-        <v>1.7520000000000001E-2</v>
+        <v>1.805E-2</v>
       </c>
       <c r="P42" s="143" t="b">
         <v>1</v>
@@ -5839,11 +5837,11 @@
       </c>
       <c r="S42" s="145">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M42,Trigger),"--")</f>
-        <v>42257</v>
+        <v>42321</v>
       </c>
       <c r="T42" s="145">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M42,Trigger),"--")</f>
-        <v>44449</v>
+        <v>44515</v>
       </c>
       <c r="V42" s="3" t="str">
         <f t="shared" si="12"/>
@@ -5908,7 +5906,7 @@
       </c>
       <c r="J43" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H43,,B43,JoinCalendar,USDSTD!D43,USDSTD!E43,USDSTD!F43,USDSTD!G43,USDSTD!I43,USDSTD!C43,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0032c#0001</v>
+        <v>obj_0030e#0001</v>
       </c>
       <c r="L43" s="69" t="str">
         <f t="shared" si="10"/>
@@ -5916,7 +5914,7 @@
       </c>
       <c r="M43" s="142" t="str">
         <f t="shared" si="11"/>
-        <v>obj_0032a#0001</v>
+        <v>obj_0030f#0001</v>
       </c>
       <c r="N43" s="151" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M43,Trigger),"--")</f>
@@ -5924,7 +5922,7 @@
       </c>
       <c r="O43" s="144">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M43,Trigger),"--")</f>
-        <v>1.9020000000000002E-2</v>
+        <v>1.9340000000000003E-2</v>
       </c>
       <c r="P43" s="143" t="b">
         <v>1</v>
@@ -5937,11 +5935,11 @@
       </c>
       <c r="S43" s="145">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M43,Trigger),"--")</f>
-        <v>42257</v>
+        <v>42321</v>
       </c>
       <c r="T43" s="145">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M43,Trigger),"--")</f>
-        <v>44816</v>
+        <v>44879</v>
       </c>
       <c r="V43" s="3" t="str">
         <f t="shared" si="12"/>
@@ -6006,7 +6004,7 @@
       </c>
       <c r="J44" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H44,,B44,JoinCalendar,USDSTD!D44,USDSTD!E44,USDSTD!F44,USDSTD!G44,USDSTD!I44,USDSTD!C44,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00329#0001</v>
+        <v>obj_0030d#0001</v>
       </c>
       <c r="L44" s="69" t="str">
         <f t="shared" si="10"/>
@@ -6014,7 +6012,7 @@
       </c>
       <c r="M44" s="142" t="str">
         <f t="shared" si="11"/>
-        <v>obj_00325#0001</v>
+        <v>obj_00319#0001</v>
       </c>
       <c r="N44" s="151" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M44,Trigger),"--")</f>
@@ -6022,7 +6020,7 @@
       </c>
       <c r="O44" s="144">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M44,Trigger),"--")</f>
-        <v>2.0219999999999998E-2</v>
+        <v>2.0400000000000001E-2</v>
       </c>
       <c r="P44" s="143" t="b">
         <v>1</v>
@@ -6035,11 +6033,11 @@
       </c>
       <c r="S44" s="145">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M44,Trigger),"--")</f>
-        <v>42257</v>
+        <v>42321</v>
       </c>
       <c r="T44" s="145">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M44,Trigger),"--")</f>
-        <v>45180</v>
+        <v>45243</v>
       </c>
       <c r="V44" s="3" t="str">
         <f t="shared" si="12"/>
@@ -6104,7 +6102,7 @@
       </c>
       <c r="J45" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H45,,B45,JoinCalendar,USDSTD!D45,USDSTD!E45,USDSTD!F45,USDSTD!G45,USDSTD!I45,USDSTD!C45,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0032b#0001</v>
+        <v>obj_00318#0001</v>
       </c>
       <c r="L45" s="69" t="str">
         <f t="shared" si="10"/>
@@ -6112,7 +6110,7 @@
       </c>
       <c r="M45" s="142" t="str">
         <f t="shared" si="11"/>
-        <v>obj_0032d#0001</v>
+        <v>obj_00310#0001</v>
       </c>
       <c r="N45" s="151" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M45,Trigger),"--")</f>
@@ -6120,7 +6118,7 @@
       </c>
       <c r="O45" s="144">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M45,Trigger),"--")</f>
-        <v>2.1219999999999999E-2</v>
+        <v>2.128E-2</v>
       </c>
       <c r="P45" s="143" t="b">
         <v>1</v>
@@ -6133,11 +6131,11 @@
       </c>
       <c r="S45" s="145">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M45,Trigger),"--")</f>
-        <v>42257</v>
+        <v>42321</v>
       </c>
       <c r="T45" s="145">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M45,Trigger),"--")</f>
-        <v>45545</v>
+        <v>45609</v>
       </c>
       <c r="V45" s="3" t="str">
         <f t="shared" si="12"/>
@@ -6202,7 +6200,7 @@
       </c>
       <c r="J46" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H46,,B46,JoinCalendar,USDSTD!D46,USDSTD!E46,USDSTD!F46,USDSTD!G46,USDSTD!I46,USDSTD!C46,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00331#0001</v>
+        <v>obj_0031c#0001</v>
       </c>
       <c r="L46" s="69" t="str">
         <f t="shared" si="10"/>
@@ -6210,7 +6208,7 @@
       </c>
       <c r="M46" s="142" t="str">
         <f t="shared" si="11"/>
-        <v>obj_00330#0001</v>
+        <v>obj_00314#0001</v>
       </c>
       <c r="N46" s="151" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M46,Trigger),"--")</f>
@@ -6218,7 +6216,7 @@
       </c>
       <c r="O46" s="144">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M46,Trigger),"--")</f>
-        <v>2.205E-2</v>
+        <v>2.2029999999999998E-2</v>
       </c>
       <c r="P46" s="143" t="b">
         <v>1</v>
@@ -6231,11 +6229,11 @@
       </c>
       <c r="S46" s="145">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M46,Trigger),"--")</f>
-        <v>42257</v>
+        <v>42321</v>
       </c>
       <c r="T46" s="145">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M46,Trigger),"--")</f>
-        <v>45910</v>
+        <v>45974</v>
       </c>
       <c r="V46" s="3" t="str">
         <f t="shared" si="12"/>
@@ -6300,7 +6298,7 @@
       </c>
       <c r="J47" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H47,,B47,JoinCalendar,USDSTD!D47,USDSTD!E47,USDSTD!F47,USDSTD!G47,USDSTD!I47,USDSTD!C47,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0032a#0001</v>
+        <v>obj_0030f#0001</v>
       </c>
       <c r="L47" s="69" t="str">
         <f t="shared" si="10"/>
@@ -6398,7 +6396,7 @@
       </c>
       <c r="J48" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H48,,B48,JoinCalendar,USDSTD!D48,USDSTD!E48,USDSTD!F48,USDSTD!G48,USDSTD!I48,USDSTD!C48,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00325#0001</v>
+        <v>obj_00319#0001</v>
       </c>
       <c r="L48" s="69" t="str">
         <f t="shared" si="10"/>
@@ -6406,7 +6404,7 @@
       </c>
       <c r="M48" s="143" t="str">
         <f t="shared" si="11"/>
-        <v>obj_00327#0001</v>
+        <v>obj_00317#0001</v>
       </c>
       <c r="N48" s="151" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M48,Trigger),"--")</f>
@@ -6414,7 +6412,7 @@
       </c>
       <c r="O48" s="144">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M48,Trigger),"--")</f>
-        <v>2.3370000000000002E-2</v>
+        <v>2.3279999999999999E-2</v>
       </c>
       <c r="P48" s="143" t="b">
         <v>1</v>
@@ -6427,11 +6425,11 @@
       </c>
       <c r="S48" s="145">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M48,Trigger),"--")</f>
-        <v>42257</v>
+        <v>42321</v>
       </c>
       <c r="T48" s="145">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M48,Trigger),"--")</f>
-        <v>46640</v>
+        <v>46706</v>
       </c>
       <c r="V48" s="3" t="str">
         <f t="shared" si="12"/>
@@ -6496,7 +6494,7 @@
       </c>
       <c r="J49" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H49,,B49,JoinCalendar,USDSTD!D49,USDSTD!E49,USDSTD!F49,USDSTD!G49,USDSTD!I49,USDSTD!C49,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0032d#0001</v>
+        <v>obj_00310#0001</v>
       </c>
       <c r="L49" s="69" t="str">
         <f t="shared" si="10"/>
@@ -6594,7 +6592,7 @@
       </c>
       <c r="J50" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H50,,B50,JoinCalendar,USDSTD!D50,USDSTD!E50,USDSTD!F50,USDSTD!G50,USDSTD!I50,USDSTD!C50,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00330#0001</v>
+        <v>obj_00314#0001</v>
       </c>
       <c r="L50" s="69" t="str">
         <f t="shared" si="10"/>
@@ -6697,7 +6695,7 @@
       </c>
       <c r="M51" s="143" t="str">
         <f t="shared" si="11"/>
-        <v>obj_00324#0001</v>
+        <v>obj_00316#0001</v>
       </c>
       <c r="N51" s="151" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M51,Trigger),"--")</f>
@@ -6705,7 +6703,7 @@
       </c>
       <c r="O51" s="144">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M51,Trigger),"--")</f>
-        <v>2.469E-2</v>
+        <v>2.452E-2</v>
       </c>
       <c r="P51" s="143" t="b">
         <v>1</v>
@@ -6718,11 +6716,11 @@
       </c>
       <c r="S51" s="145">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M51,Trigger),"--")</f>
-        <v>42257</v>
+        <v>42321</v>
       </c>
       <c r="T51" s="145">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M51,Trigger),"--")</f>
-        <v>47736</v>
+        <v>47800</v>
       </c>
       <c r="V51" s="3" t="str">
         <f t="shared" si="12"/>
@@ -6787,7 +6785,7 @@
       </c>
       <c r="J52" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H52,,B52,JoinCalendar,USDSTD!D52,USDSTD!E52,USDSTD!F52,USDSTD!G52,USDSTD!I52,USDSTD!C52,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00327#0001</v>
+        <v>obj_00317#0001</v>
       </c>
       <c r="L52" s="69" t="str">
         <f t="shared" si="10"/>
@@ -7075,7 +7073,7 @@
       </c>
       <c r="J55" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H55,,B55,JoinCalendar,USDSTD!D55,USDSTD!E55,USDSTD!F55,USDSTD!G55,USDSTD!I55,USDSTD!C55,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00324#0001</v>
+        <v>obj_00316#0001</v>
       </c>
       <c r="L55" s="69" t="str">
         <f t="shared" si="10"/>
@@ -7178,7 +7176,7 @@
       </c>
       <c r="M56" s="143" t="str">
         <f t="shared" si="11"/>
-        <v>obj_00332#0001</v>
+        <v>obj_00311#0001</v>
       </c>
       <c r="N56" s="151" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M56,Trigger),"--")</f>
@@ -7186,7 +7184,7 @@
       </c>
       <c r="O56" s="144">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M56,Trigger),"--")</f>
-        <v>2.589E-2</v>
+        <v>2.5770000000000001E-2</v>
       </c>
       <c r="P56" s="143" t="b">
         <v>1</v>
@@ -7199,11 +7197,11 @@
       </c>
       <c r="S56" s="145">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M56,Trigger),"--")</f>
-        <v>42257</v>
+        <v>42321</v>
       </c>
       <c r="T56" s="145">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M56,Trigger),"--")</f>
-        <v>49562</v>
+        <v>49626</v>
       </c>
       <c r="V56" s="3" t="str">
         <f t="shared" si="12"/>
@@ -7553,7 +7551,7 @@
       </c>
       <c r="J60" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H60,,B60,JoinCalendar,USDSTD!D60,USDSTD!E60,USDSTD!F60,USDSTD!G60,USDSTD!I60,USDSTD!C60,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00332#0001</v>
+        <v>obj_00311#0001</v>
       </c>
       <c r="L60" s="69" t="str">
         <f t="shared" si="10"/>
@@ -7656,7 +7654,7 @@
       </c>
       <c r="M61" s="143" t="str">
         <f t="shared" si="11"/>
-        <v>obj_0032e#0001</v>
+        <v>obj_00313#0001</v>
       </c>
       <c r="N61" s="151" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M61,Trigger),"--")</f>
@@ -7664,7 +7662,7 @@
       </c>
       <c r="O61" s="144">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M61,Trigger),"--")</f>
-        <v>2.648E-2</v>
+        <v>2.6309999999999997E-2</v>
       </c>
       <c r="P61" s="143" t="b">
         <v>1</v>
@@ -7677,11 +7675,11 @@
       </c>
       <c r="S61" s="145">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M61,Trigger),"--")</f>
-        <v>42257</v>
+        <v>42321</v>
       </c>
       <c r="T61" s="145">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M61,Trigger),"--")</f>
-        <v>51389</v>
+        <v>51453</v>
       </c>
       <c r="V61" s="3" t="str">
         <f t="shared" si="12"/>
@@ -8031,7 +8029,7 @@
       </c>
       <c r="J65" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H65,,B65,JoinCalendar,USDSTD!D65,USDSTD!E65,USDSTD!F65,USDSTD!G65,USDSTD!I65,USDSTD!C65,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0032e#0001</v>
+        <v>obj_00313#0001</v>
       </c>
       <c r="L65" s="69" t="str">
         <f t="shared" si="10"/>
@@ -8134,7 +8132,7 @@
       </c>
       <c r="M66" s="143" t="str">
         <f t="shared" si="11"/>
-        <v>obj_0032f#0001</v>
+        <v>obj_0031b#0001</v>
       </c>
       <c r="N66" s="151" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M66,Trigger),"--")</f>
@@ -8142,7 +8140,7 @@
       </c>
       <c r="O66" s="144">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M66,Trigger),"--")</f>
-        <v>2.6839999999999996E-2</v>
+        <v>2.6619999999999998E-2</v>
       </c>
       <c r="P66" s="143" t="b">
         <v>1</v>
@@ -8155,11 +8153,11 @@
       </c>
       <c r="S66" s="145">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M66,Trigger),"--")</f>
-        <v>42257</v>
+        <v>42321</v>
       </c>
       <c r="T66" s="145">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M66,Trigger),"--")</f>
-        <v>53216</v>
+        <v>53279</v>
       </c>
       <c r="V66" s="3" t="str">
         <f t="shared" si="12"/>
@@ -8324,19 +8322,19 @@
       </c>
       <c r="M68" s="143" t="str">
         <f t="shared" si="11"/>
-        <v>obj_00326#0001</v>
+        <v>obj_00312#0001</v>
       </c>
       <c r="N68" s="151" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M68,Trigger),"--")</f>
         <v>USDAM3L40Y_Quote</v>
       </c>
-      <c r="O68" s="144" t="str">
+      <c r="O68" s="144">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M68,Trigger),"--")</f>
-        <v>--</v>
-      </c>
-      <c r="P68" s="165" t="b">
+        <v>2.6789999999999998E-2</v>
+      </c>
+      <c r="P68" s="163" t="b">
         <f>NOT(ISERROR(_xll.qlQuoteValue(N68)))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q68" s="143">
         <v>50</v>
@@ -8346,11 +8344,11 @@
       </c>
       <c r="S68" s="145">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M68,Trigger),"--")</f>
-        <v>42257</v>
+        <v>42321</v>
       </c>
       <c r="T68" s="145">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M68,Trigger),"--")</f>
-        <v>56867</v>
+        <v>56933</v>
       </c>
       <c r="V68" s="3" t="str">
         <f t="shared" si="12"/>
@@ -8510,7 +8508,7 @@
       </c>
       <c r="J70" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H70,,B70,JoinCalendar,USDSTD!D70,USDSTD!E70,USDSTD!F70,USDSTD!G70,USDSTD!I70,USDSTD!C70,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0032f#0001</v>
+        <v>obj_0031b#0001</v>
       </c>
       <c r="L70" s="69" t="str">
         <f t="shared" si="10"/>
@@ -8518,19 +8516,19 @@
       </c>
       <c r="M70" s="143" t="str">
         <f t="shared" si="11"/>
-        <v>obj_00328#0001</v>
+        <v>obj_0031a#0001</v>
       </c>
       <c r="N70" s="151" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M70,Trigger),"--")</f>
         <v>USDAM3L50Y_Quote</v>
       </c>
-      <c r="O70" s="144" t="str">
+      <c r="O70" s="144">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M70,Trigger),"--")</f>
-        <v>--</v>
-      </c>
-      <c r="P70" s="165" t="b">
+        <v>2.6670000000000003E-2</v>
+      </c>
+      <c r="P70" s="163" t="b">
         <f>NOT(ISERROR(_xll.qlQuoteValue(N70)))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q70" s="143">
         <v>50</v>
@@ -8540,11 +8538,11 @@
       </c>
       <c r="S70" s="145">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M70,Trigger),"--")</f>
-        <v>42257</v>
+        <v>42321</v>
       </c>
       <c r="T70" s="145">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M70,Trigger),"--")</f>
-        <v>60520</v>
+        <v>60584</v>
       </c>
       <c r="V70" s="3" t="str">
         <f t="shared" si="12"/>
@@ -8614,7 +8612,7 @@
       </c>
       <c r="M71" s="146" t="str">
         <f t="shared" si="11"/>
-        <v>obj_00333#0001</v>
+        <v>obj_00315#0001</v>
       </c>
       <c r="N71" s="156" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M71,Trigger),"--")</f>
@@ -8635,11 +8633,11 @@
       </c>
       <c r="S71" s="155">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M71,Trigger),"--")</f>
-        <v>42257</v>
+        <v>42321</v>
       </c>
       <c r="T71" s="155">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M71,Trigger),"--")</f>
-        <v>64172</v>
+        <v>64236</v>
       </c>
       <c r="V71" s="5" t="str">
         <f t="shared" si="12"/>
@@ -8704,7 +8702,7 @@
       </c>
       <c r="J72" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H72,,B72,JoinCalendar,USDSTD!D72,USDSTD!E72,USDSTD!F72,USDSTD!G72,USDSTD!I72,USDSTD!C72,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00326#0001</v>
+        <v>obj_00312#0001</v>
       </c>
     </row>
     <row r="73" spans="1:29" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8771,7 +8769,7 @@
       </c>
       <c r="J74" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H74,,B74,JoinCalendar,USDSTD!D74,USDSTD!E74,USDSTD!F74,USDSTD!G74,USDSTD!I74,USDSTD!C74,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00328#0001</v>
+        <v>obj_0031a#0001</v>
       </c>
     </row>
     <row r="75" spans="1:29" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8806,7 +8804,7 @@
       </c>
       <c r="J75" s="2" t="str">
         <f>_xll.qlSwapRateHelper2(,H75,,B75,JoinCalendar,USDSTD!D75,USDSTD!E75,USDSTD!F75,USDSTD!G75,USDSTD!I75,USDSTD!C75,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00333#0001</v>
+        <v>obj_00315#0001</v>
       </c>
     </row>
     <row r="76" spans="1:29" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
USD Contribution with FuturesRollTest + USD STD with extrapolation
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/USD/USD_YCSTDBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/USD/USD_YCSTDBootstrapping.xlsx
@@ -1618,7 +1618,7 @@
       </c>
       <c r="I3" s="13">
         <f>_xll.qlSettingsEvaluationDate(Trigger)</f>
-        <v>42318</v>
+        <v>42345</v>
       </c>
       <c r="J3" s="83"/>
     </row>
@@ -1637,7 +1637,7 @@
       </c>
       <c r="I4" s="15">
         <f>_xll.qlCalendarAdvance(Calendar,Evaluationdate,"2D","F",,Trigger)</f>
-        <v>42320</v>
+        <v>42347</v>
       </c>
       <c r="J4" s="83"/>
     </row>
@@ -1778,7 +1778,7 @@
       </c>
       <c r="D14" s="41" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D16,D17,LocalCalendar,_xll.ohPack(USDSTD!W3:W71),,,,D18,D19,D20,Permanent,,ObjectOverwrite)</f>
-        <v>_USDSTD#0002</v>
+        <v>_USDSTD#0001</v>
       </c>
       <c r="E14" s="42"/>
     </row>
@@ -1851,7 +1851,7 @@
       <c r="B22" s="23"/>
       <c r="C22" s="32">
         <f>_xll.qlTermStructureReferenceDate(YieldCurve_STD)</f>
-        <v>42318</v>
+        <v>42345</v>
       </c>
       <c r="D22" s="33">
         <f>_xll.qlYieldTSDiscount(YieldCurve_STD,C22,,Trigger)</f>
@@ -1863,11 +1863,11 @@
       <c r="B23" s="23"/>
       <c r="C23" s="34">
         <f>_xll.qlTermStructureMaxDate(YieldCurve_STD,Trigger)</f>
-        <v>60584</v>
+        <v>60610</v>
       </c>
       <c r="D23" s="35">
         <f>_xll.qlYieldTSDiscount(YieldCurve_STD,C23,,Trigger)</f>
-        <v>0.25664810096502239</v>
+        <v>0.2668285180219151</v>
       </c>
       <c r="E23" s="42"/>
     </row>
@@ -1889,7 +1889,8 @@
         <v>116</v>
       </c>
       <c r="D25" s="37" t="b">
-        <v>0</v>
+        <f>_xll.qlExtrapolatorEnableExtrapolation(YieldCurve_STD,TRUE)</f>
+        <v>1</v>
       </c>
       <c r="E25" s="42"/>
     </row>
@@ -2086,7 +2087,7 @@
       </c>
       <c r="AC2" s="160">
         <f t="array" ref="AC2:AC71">_xll.qlPiecewiseYieldCurveData(YieldCurve_STD,Trigger)</f>
-        <v>2.9402540924823879E-3</v>
+        <v>2.7374897344519516E-3</v>
       </c>
       <c r="AE2" s="164" t="s">
         <v>84</v>
@@ -2109,7 +2110,7 @@
       <c r="F3" s="125"/>
       <c r="G3" s="114" t="str">
         <f>_xll.qlLibor(,Currency,C3,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00306#0001</v>
+        <v>obj_00305#0001</v>
       </c>
       <c r="H3" s="122" t="str">
         <f t="shared" ref="H3:H11" si="0">Currency&amp;$B3&amp;"D"&amp;$H$1&amp;QuoteSuffix</f>
@@ -2118,7 +2119,7 @@
       <c r="I3" s="125"/>
       <c r="J3" s="115" t="str">
         <f>_xll.qlDepositRateHelper(,H3,G3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0030a#0001</v>
+        <v>obj_00308#0001</v>
       </c>
       <c r="K3" s="49"/>
       <c r="L3" s="66" t="str">
@@ -2127,7 +2128,7 @@
       </c>
       <c r="M3" s="133" t="str">
         <f>IF(ISBLANK(J3),"--",J3)</f>
-        <v>obj_0030a#0001</v>
+        <v>obj_00308#0001</v>
       </c>
       <c r="N3" s="147" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M3,Trigger),"--")</f>
@@ -2135,7 +2136,7 @@
       </c>
       <c r="O3" s="135">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M3,Trigger),"--")</f>
-        <v>2.8999999999999998E-3</v>
+        <v>2.7000000000000001E-3</v>
       </c>
       <c r="P3" s="134" t="b">
         <v>1</v>
@@ -2148,11 +2149,11 @@
       </c>
       <c r="S3" s="136">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M3,Trigger),"--")</f>
-        <v>42318</v>
+        <v>42345</v>
       </c>
       <c r="T3" s="136">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M3,Trigger),"--")</f>
-        <v>42320</v>
+        <v>42346</v>
       </c>
       <c r="V3" s="3" t="str">
         <f t="shared" ref="V3:V34" si="1">IFERROR(INDEX($L$3:$L$71,MATCH(X3,$N$3:$N$71,0),1),"")</f>
@@ -2160,7 +2161,7 @@
       </c>
       <c r="W3" s="3" t="str">
         <f t="array" ref="W3:W71">_xll.qlRateHelperSelection(_xll.ohFilter(RateHelpers,IncludeFlag),_xll.ohFilter(Priority,IncludeFlag),$AF$3,$AF$4,$AF$5,$AF$6,_xll.ohFilter(MinDistance,IncludeFlag),Trigger)</f>
-        <v>obj_0030a</v>
+        <v>obj_00308</v>
       </c>
       <c r="X3" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W3,Trigger),"")</f>
@@ -2168,7 +2169,7 @@
       </c>
       <c r="Y3" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W3,Trigger),"")</f>
-        <v>2.8999999999999998E-3</v>
+        <v>2.7000000000000001E-3</v>
       </c>
       <c r="Z3" s="105" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W3)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W3)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W3)),_xll.qlSwapRateHelperSpread($W3))</f>
@@ -2176,14 +2177,14 @@
       </c>
       <c r="AA3" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W3,Trigger),"")</f>
-        <v>42318</v>
+        <v>42345</v>
       </c>
       <c r="AB3" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W3,Trigger),"")</f>
-        <v>42320</v>
+        <v>42346</v>
       </c>
       <c r="AC3" s="68">
-        <v>2.9402540924823879E-3</v>
+        <v>2.7374897344519516E-3</v>
       </c>
       <c r="AE3" s="108" t="s">
         <v>85</v>
@@ -2217,7 +2218,7 @@
       <c r="I4" s="132"/>
       <c r="J4" s="57" t="str">
         <f>_xll.qlFraRateHelper(,H4,"1D",G4,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00307#0001</v>
+        <v>obj_00306#0001</v>
       </c>
       <c r="K4" s="48"/>
       <c r="L4" s="9" t="str">
@@ -2226,7 +2227,7 @@
       </c>
       <c r="M4" s="95" t="str">
         <f t="shared" ref="M4:M11" si="3">IF(ISBLANK(J4),"--",J4)</f>
-        <v>obj_00307#0001</v>
+        <v>obj_00306#0001</v>
       </c>
       <c r="N4" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M4,Trigger),"--")</f>
@@ -2234,7 +2235,7 @@
       </c>
       <c r="O4" s="99">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M4,Trigger),"--")</f>
-        <v>2.8999999999999998E-3</v>
+        <v>2.7000000000000001E-3</v>
       </c>
       <c r="P4" s="98" t="b">
         <v>1</v>
@@ -2247,18 +2248,18 @@
       </c>
       <c r="S4" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M4,Trigger),"--")</f>
-        <v>42320</v>
+        <v>42346</v>
       </c>
       <c r="T4" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M4,Trigger),"--")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="V4" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Dp</v>
       </c>
       <c r="W4" s="3" t="str">
-        <v>obj_00307</v>
+        <v>obj_00306</v>
       </c>
       <c r="X4" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W4,Trigger),"")</f>
@@ -2266,7 +2267,7 @@
       </c>
       <c r="Y4" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W4,Trigger),"")</f>
-        <v>2.8999999999999998E-3</v>
+        <v>2.7000000000000001E-3</v>
       </c>
       <c r="Z4" s="105" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W4)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W4)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W4)),_xll.qlSwapRateHelperSpread($W4))</f>
@@ -2274,14 +2275,14 @@
       </c>
       <c r="AA4" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W4,Trigger),"")</f>
-        <v>42320</v>
+        <v>42346</v>
       </c>
       <c r="AB4" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W4,Trigger),"")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="AC4" s="68">
-        <v>2.9402580400256706E-3</v>
+        <v>2.7374897344653723E-3</v>
       </c>
       <c r="AE4" s="108" t="s">
         <v>86</v>
@@ -2306,7 +2307,7 @@
       <c r="F5" s="127"/>
       <c r="G5" s="6" t="str">
         <f>_xll.qlLibor(,Currency,C5,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00304#0001</v>
+        <v>obj_00303#0001</v>
       </c>
       <c r="H5" s="124" t="str">
         <f t="shared" si="0"/>
@@ -2315,7 +2316,7 @@
       <c r="I5" s="127"/>
       <c r="J5" s="2" t="str">
         <f>_xll.qlFraRateHelper(,H5,"2D",G5,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00309#0001</v>
+        <v>obj_0030b#0001</v>
       </c>
       <c r="K5" s="48"/>
       <c r="L5" s="9" t="str">
@@ -2324,7 +2325,7 @@
       </c>
       <c r="M5" s="95" t="str">
         <f t="shared" si="3"/>
-        <v>obj_00309#0001</v>
+        <v>obj_0030b#0001</v>
       </c>
       <c r="N5" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M5,Trigger),"--")</f>
@@ -2332,7 +2333,7 @@
       </c>
       <c r="O5" s="99">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M5,Trigger),"--")</f>
-        <v>3.0000000000000001E-3</v>
+        <v>2.7000000000000001E-3</v>
       </c>
       <c r="P5" s="98" t="b">
         <v>1</v>
@@ -2345,18 +2346,18 @@
       </c>
       <c r="S5" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M5,Trigger),"--")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="T5" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M5,Trigger),"--")</f>
-        <v>42324</v>
+        <v>42348</v>
       </c>
       <c r="V5" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Dp</v>
       </c>
       <c r="W5" s="3" t="str">
-        <v>obj_00309</v>
+        <v>obj_0030b</v>
       </c>
       <c r="X5" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W5,Trigger),"")</f>
@@ -2364,7 +2365,7 @@
       </c>
       <c r="Y5" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W5,Trigger),"")</f>
-        <v>3.0000000000000001E-3</v>
+        <v>2.7000000000000001E-3</v>
       </c>
       <c r="Z5" s="105" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W5)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W5)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W5)),_xll.qlSwapRateHelperSpread($W5))</f>
@@ -2372,14 +2373,14 @@
       </c>
       <c r="AA5" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W5,Trigger),"")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="AB5" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W5,Trigger),"")</f>
-        <v>42324</v>
+        <v>42348</v>
       </c>
       <c r="AC5" s="68">
-        <v>2.9909433432465256E-3</v>
+        <v>2.7374897344756778E-3</v>
       </c>
       <c r="AD5" s="76"/>
       <c r="AE5" s="108" t="s">
@@ -2406,7 +2407,7 @@
       <c r="F6" s="126"/>
       <c r="G6" s="60" t="str">
         <f>_xll.qlLibor(,Currency,C6,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00303#0001</v>
+        <v>obj_00302#0001</v>
       </c>
       <c r="H6" s="123" t="str">
         <f t="shared" si="0"/>
@@ -2415,7 +2416,7 @@
       <c r="I6" s="126"/>
       <c r="J6" s="62" t="str">
         <f>_xll.qlDepositRateHelper(,H6,G6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00308#0001</v>
+        <v>obj_0030a#0001</v>
       </c>
       <c r="K6" s="48"/>
       <c r="L6" s="9" t="str">
@@ -2424,7 +2425,7 @@
       </c>
       <c r="M6" s="95" t="str">
         <f t="shared" si="3"/>
-        <v>obj_00308#0001</v>
+        <v>obj_0030a#0001</v>
       </c>
       <c r="N6" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M6,Trigger),"--")</f>
@@ -2432,7 +2433,7 @@
       </c>
       <c r="O6" s="99">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M6,Trigger),"--")</f>
-        <v>1.5560000000000001E-3</v>
+        <v>1.5845E-3</v>
       </c>
       <c r="P6" s="98" t="b">
         <v>1</v>
@@ -2445,18 +2446,18 @@
       </c>
       <c r="S6" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M6,Trigger),"--")</f>
-        <v>42320</v>
+        <v>42347</v>
       </c>
       <c r="T6" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M6,Trigger),"--")</f>
-        <v>42327</v>
+        <v>42354</v>
       </c>
       <c r="V6" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Dp</v>
       </c>
       <c r="W6" s="3" t="str">
-        <v>obj_00308</v>
+        <v>obj_0030a</v>
       </c>
       <c r="X6" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W6,Trigger),"")</f>
@@ -2464,7 +2465,7 @@
       </c>
       <c r="Y6" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W6,Trigger),"")</f>
-        <v>1.5560000000000001E-3</v>
+        <v>1.5845E-3</v>
       </c>
       <c r="Z6" s="105" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W6)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W6)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W6)),_xll.qlSwapRateHelperSpread($W6))</f>
@@ -2472,14 +2473,14 @@
       </c>
       <c r="AA6" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W6,Trigger),"")</f>
-        <v>42320</v>
+        <v>42347</v>
       </c>
       <c r="AB6" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W6,Trigger),"")</f>
-        <v>42327</v>
+        <v>42354</v>
       </c>
       <c r="AC6" s="68">
-        <v>1.8804021006482438E-3</v>
+        <v>1.8578172052717264E-3</v>
       </c>
       <c r="AE6" s="108" t="s">
         <v>88</v>
@@ -2505,7 +2506,7 @@
       <c r="F7" s="126"/>
       <c r="G7" s="60" t="str">
         <f>_xll.qlLibor(,Currency,C7,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00302#0001</v>
+        <v>obj_00301#0001</v>
       </c>
       <c r="H7" s="123" t="str">
         <f t="shared" si="0"/>
@@ -2531,7 +2532,7 @@
       </c>
       <c r="O7" s="99">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M7,Trigger),"--")</f>
-        <v>1.97E-3</v>
+        <v>2.7549999999999996E-3</v>
       </c>
       <c r="P7" s="98" t="b">
         <v>1</v>
@@ -2544,11 +2545,11 @@
       </c>
       <c r="S7" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M7,Trigger),"--")</f>
-        <v>42320</v>
+        <v>42347</v>
       </c>
       <c r="T7" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M7,Trigger),"--")</f>
-        <v>42352</v>
+        <v>42380</v>
       </c>
       <c r="V7" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2563,7 +2564,7 @@
       </c>
       <c r="Y7" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W7,Trigger),"")</f>
-        <v>1.97E-3</v>
+        <v>2.7549999999999996E-3</v>
       </c>
       <c r="Z7" s="105" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W7)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W7)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W7)),_xll.qlSwapRateHelperSpread($W7))</f>
@@ -2571,14 +2572,14 @@
       </c>
       <c r="AA7" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W7,Trigger),"")</f>
-        <v>42320</v>
+        <v>42347</v>
       </c>
       <c r="AB7" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W7,Trigger),"")</f>
-        <v>42352</v>
+        <v>42380</v>
       </c>
       <c r="AC7" s="68">
-        <v>2.052660830115613E-3</v>
+        <v>2.7897442972641558E-3</v>
       </c>
       <c r="AH7" s="161"/>
     </row>
@@ -2598,7 +2599,7 @@
       <c r="F8" s="126"/>
       <c r="G8" s="60" t="str">
         <f>_xll.qlLibor(,Currency,C8,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00305#0001</v>
+        <v>obj_00304#0001</v>
       </c>
       <c r="H8" s="123" t="str">
         <f t="shared" si="0"/>
@@ -2607,7 +2608,7 @@
       <c r="I8" s="126"/>
       <c r="J8" s="62" t="str">
         <f>_xll.qlDepositRateHelper(,H8,G8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0030b#0001</v>
+        <v>obj_00309#0001</v>
       </c>
       <c r="K8" s="48"/>
       <c r="L8" s="9" t="str">
@@ -2616,7 +2617,7 @@
       </c>
       <c r="M8" s="95" t="str">
         <f t="shared" si="3"/>
-        <v>obj_0030b#0001</v>
+        <v>obj_00309#0001</v>
       </c>
       <c r="N8" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M8,Trigger),"--")</f>
@@ -2624,7 +2625,7 @@
       </c>
       <c r="O8" s="99">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M8,Trigger),"--")</f>
-        <v>2.725E-3</v>
+        <v>3.6070000000000004E-3</v>
       </c>
       <c r="P8" s="98" t="b">
         <v>1</v>
@@ -2637,18 +2638,18 @@
       </c>
       <c r="S8" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M8,Trigger),"--")</f>
-        <v>42320</v>
+        <v>42347</v>
       </c>
       <c r="T8" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M8,Trigger),"--")</f>
-        <v>42381</v>
+        <v>42409</v>
       </c>
       <c r="V8" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Dp</v>
       </c>
       <c r="W8" s="3" t="str">
-        <v>obj_0030b</v>
+        <v>obj_00309</v>
       </c>
       <c r="X8" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W8,Trigger),"")</f>
@@ -2656,7 +2657,7 @@
       </c>
       <c r="Y8" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W8,Trigger),"")</f>
-        <v>2.725E-3</v>
+        <v>3.6070000000000004E-3</v>
       </c>
       <c r="Z8" s="105" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W8)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W8)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W8)),_xll.qlSwapRateHelperSpread($W8))</f>
@@ -2664,14 +2665,14 @@
       </c>
       <c r="AA8" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W8,Trigger),"")</f>
-        <v>42320</v>
+        <v>42347</v>
       </c>
       <c r="AB8" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W8,Trigger),"")</f>
-        <v>42381</v>
+        <v>42409</v>
       </c>
       <c r="AC8" s="68">
-        <v>2.7678617725453596E-3</v>
+        <v>3.6272595361985724E-3</v>
       </c>
       <c r="AH8" s="161"/>
     </row>
@@ -2717,7 +2718,7 @@
       </c>
       <c r="O9" s="99">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M9,Trigger),"--")</f>
-        <v>3.5560000000000001E-3</v>
+        <v>4.62E-3</v>
       </c>
       <c r="P9" s="98" t="b">
         <v>1</v>
@@ -2730,11 +2731,11 @@
       </c>
       <c r="S9" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M9,Trigger),"--")</f>
-        <v>42320</v>
+        <v>42347</v>
       </c>
       <c r="T9" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M9,Trigger),"--")</f>
-        <v>42412</v>
+        <v>42438</v>
       </c>
       <c r="V9" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2749,7 +2750,7 @@
       </c>
       <c r="Y9" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W9,Trigger),"")</f>
-        <v>3.5560000000000001E-3</v>
+        <v>4.62E-3</v>
       </c>
       <c r="Z9" s="105" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W9)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W9)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W9)),_xll.qlSwapRateHelperSpread($W9))</f>
@@ -2757,14 +2758,14 @@
       </c>
       <c r="AA9" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W9,Trigger),"")</f>
-        <v>42320</v>
+        <v>42347</v>
       </c>
       <c r="AB9" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W9,Trigger),"")</f>
-        <v>42412</v>
+        <v>42438</v>
       </c>
       <c r="AC9" s="68">
-        <v>3.589634702329533E-3</v>
+        <v>4.6396283862004256E-3</v>
       </c>
       <c r="AH9" s="161"/>
     </row>
@@ -2831,7 +2832,7 @@
         <v>FUT</v>
       </c>
       <c r="W10" s="3" t="str">
-        <v>obj_0031d</v>
+        <v>obj_0031f</v>
       </c>
       <c r="X10" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W10,Trigger),"")</f>
@@ -2839,11 +2840,11 @@
       </c>
       <c r="Y10" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W10,Trigger),"")</f>
-        <v>4.3729641797705821E-3</v>
+        <v>5.087129734291344E-3</v>
       </c>
       <c r="Z10" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W10)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W10)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W10)),_xll.qlSwapRateHelperSpread($W10))</f>
-        <v>2.0358202294357524E-6</v>
+        <v>3.7026570856742148E-7</v>
       </c>
       <c r="AA10" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W10,Trigger),"")</f>
@@ -2854,7 +2855,7 @@
         <v>42445</v>
       </c>
       <c r="AC10" s="68">
-        <v>3.770986716006456E-3</v>
+        <v>4.8577720877382982E-3</v>
       </c>
       <c r="AH10" s="161"/>
     </row>
@@ -2921,7 +2922,7 @@
         <v>FUT</v>
       </c>
       <c r="W11" s="3" t="str">
-        <v>obj_00321</v>
+        <v>obj_0031e</v>
       </c>
       <c r="X11" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W11,Trigger),"")</f>
@@ -2929,11 +2930,11 @@
       </c>
       <c r="Y11" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W11,Trigger),"")</f>
-        <v>6.0648182583541007E-3</v>
+        <v>6.768919599396443E-3</v>
       </c>
       <c r="Z11" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W11)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W11)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W11)),_xll.qlSwapRateHelperSpread($W11))</f>
-        <v>1.0181741645951506E-5</v>
+        <v>6.0804006036435164E-6</v>
       </c>
       <c r="AA11" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W11,Trigger),"")</f>
@@ -2944,7 +2945,7 @@
         <v>42537</v>
       </c>
       <c r="AC11" s="68">
-        <v>4.7679914916027759E-3</v>
+        <v>5.815737061746382E-3</v>
       </c>
       <c r="AH11" s="161"/>
     </row>
@@ -2971,11 +2972,11 @@
       </c>
       <c r="N12" s="147" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M12,Trigger),"--")</f>
-        <v>USDFUT3MX5_Quote</v>
+        <v>USDFUT3MZ5_Quote</v>
       </c>
       <c r="O12" s="152">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M12,Trigger),"--")</f>
-        <v>99.631249999999994</v>
+        <v>99.491250000000008</v>
       </c>
       <c r="P12" s="134" t="b">
         <v>1</v>
@@ -2988,11 +2989,11 @@
       </c>
       <c r="S12" s="136">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M12,Trigger),"--")</f>
-        <v>42326</v>
+        <v>42354</v>
       </c>
       <c r="T12" s="136">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M12,Trigger),"--")</f>
-        <v>42418</v>
+        <v>42445</v>
       </c>
       <c r="V12" s="3" t="str">
         <f t="shared" si="1"/>
@@ -3007,11 +3008,11 @@
       </c>
       <c r="Y12" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W12,Trigger),"")</f>
-        <v>7.602558496357415E-3</v>
+        <v>8.3597653325650362E-3</v>
       </c>
       <c r="Z12" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W12)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W12)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W12)),_xll.qlSwapRateHelperSpread($W12))</f>
-        <v>2.2441503642577717E-5</v>
+        <v>1.5234667434985482E-5</v>
       </c>
       <c r="AA12" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W12,Trigger),"")</f>
@@ -3022,7 +3023,7 @@
         <v>42628</v>
       </c>
       <c r="AC12" s="68">
-        <v>5.6307143072360484E-3</v>
+        <v>6.6705495488256711E-3</v>
       </c>
       <c r="AH12" s="161"/>
     </row>
@@ -3062,11 +3063,11 @@
       </c>
       <c r="N13" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M13,Trigger),"--")</f>
-        <v>USDFUT3MZ5_Quote</v>
+        <v>USDFUT3MF6_Quote</v>
       </c>
       <c r="O13" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M13,Trigger),"--")</f>
-        <v>99.5625</v>
+        <v>99.422499999999999</v>
       </c>
       <c r="P13" s="98" t="b">
         <v>1</v>
@@ -3079,11 +3080,11 @@
       </c>
       <c r="S13" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M13,Trigger),"--")</f>
-        <v>42354</v>
+        <v>42389</v>
       </c>
       <c r="T13" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M13,Trigger),"--")</f>
-        <v>42445</v>
+        <v>42480</v>
       </c>
       <c r="V13" s="3" t="str">
         <f t="shared" si="1"/>
@@ -3098,11 +3099,11 @@
       </c>
       <c r="Y13" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W13,Trigger),"")</f>
-        <v>9.3349948777573678E-3</v>
+        <v>9.9962575268070491E-3</v>
       </c>
       <c r="Z13" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W13)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W13)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W13)),_xll.qlSwapRateHelperSpread($W13))</f>
-        <v>4.0005122242654754E-5</v>
+        <v>2.8742473192902007E-5</v>
       </c>
       <c r="AA13" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W13,Trigger),"")</f>
@@ -3113,7 +3114,7 @@
         <v>42725</v>
       </c>
       <c r="AC13" s="68">
-        <v>6.5285594706942767E-3</v>
+        <v>7.5379611371936949E-3</v>
       </c>
       <c r="AH13" s="161"/>
     </row>
@@ -3126,7 +3127,7 @@
       </c>
       <c r="C14" s="56" t="str">
         <f>_xll.qlIMMNextCode(Evaluationdate-1,B14,Trigger)</f>
-        <v>X5</v>
+        <v>Z5</v>
       </c>
       <c r="D14" s="132"/>
       <c r="E14" s="132"/>
@@ -3137,11 +3138,11 @@
       </c>
       <c r="H14" s="119" t="str">
         <f t="shared" ref="H14:H35" si="8">Currency&amp;"FUT"&amp;$G$1&amp;$C14&amp;QuoteSuffix</f>
-        <v>USDFUT3MX5_Quote</v>
+        <v>USDFUT3MZ5_Quote</v>
       </c>
       <c r="I14" s="119" t="str">
         <f t="shared" ref="I14:I35" si="9">Currency&amp;"FUT"&amp;$G$1&amp;$C14&amp;"ConvAdj"&amp;QuoteSuffix</f>
-        <v>USDFUT3MX5ConvAdj_Quote</v>
+        <v>USDFUT3MZ5ConvAdj_Quote</v>
       </c>
       <c r="J14" s="57" t="str">
         <f>_xll.qlFuturesRateHelper(,H14,$H$12,C14,G14,I14,Permanent,Trigger,ObjectOverwrite)</f>
@@ -3158,11 +3159,11 @@
       </c>
       <c r="N14" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M14,Trigger),"--")</f>
-        <v>USDFUT3MF6_Quote</v>
+        <v>USDFUT3MG6_Quote</v>
       </c>
       <c r="O14" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M14,Trigger),"--")</f>
-        <v>99.492500000000007</v>
+        <v>99.377499999999998</v>
       </c>
       <c r="P14" s="98" t="b">
         <v>1</v>
@@ -3175,11 +3176,11 @@
       </c>
       <c r="S14" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M14,Trigger),"--")</f>
-        <v>42389</v>
+        <v>42417</v>
       </c>
       <c r="T14" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M14,Trigger),"--")</f>
-        <v>42480</v>
+        <v>42507</v>
       </c>
       <c r="V14" s="3" t="str">
         <f t="shared" si="1"/>
@@ -3194,11 +3195,11 @@
       </c>
       <c r="Y14" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W14,Trigger),"")</f>
-        <v>1.1064680754560763E-2</v>
+        <v>1.1680372313889501E-2</v>
       </c>
       <c r="Z14" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W14)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W14)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W14)),_xll.qlSwapRateHelperSpread($W14))</f>
-        <v>6.0319245439177848E-5</v>
+        <v>4.4627686110485285E-5</v>
       </c>
       <c r="AA14" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W14,Trigger),"")</f>
@@ -3209,7 +3210,7 @@
         <v>42815</v>
       </c>
       <c r="AC14" s="68">
-        <v>7.375014000973029E-3</v>
+        <v>8.3589490667817946E-3</v>
       </c>
       <c r="AH14" s="161"/>
     </row>
@@ -3222,7 +3223,7 @@
       </c>
       <c r="C15" s="61" t="str">
         <f>_xll.qlIMMNextCode(C14,B15,Trigger)</f>
-        <v>Z5</v>
+        <v>F6</v>
       </c>
       <c r="D15" s="126"/>
       <c r="E15" s="126"/>
@@ -3233,11 +3234,11 @@
       </c>
       <c r="H15" s="120" t="str">
         <f t="shared" si="8"/>
-        <v>USDFUT3MZ5_Quote</v>
+        <v>USDFUT3MF6_Quote</v>
       </c>
       <c r="I15" s="120" t="str">
         <f t="shared" si="9"/>
-        <v>USDFUT3MZ5ConvAdj_Quote</v>
+        <v>USDFUT3MF6ConvAdj_Quote</v>
       </c>
       <c r="J15" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H15,$H$12,C15,G15,I15,Permanent,Trigger,ObjectOverwrite)</f>
@@ -3254,11 +3255,11 @@
       </c>
       <c r="N15" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M15,Trigger),"--")</f>
-        <v>USDFUT3MG6_Quote</v>
+        <v>USDFUT3MH6_Quote</v>
       </c>
       <c r="O15" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M15,Trigger),"--")</f>
-        <v>99.4375</v>
+        <v>99.322499999999991</v>
       </c>
       <c r="P15" s="98" t="b">
         <v>1</v>
@@ -3271,11 +3272,11 @@
       </c>
       <c r="S15" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M15,Trigger),"--")</f>
-        <v>42417</v>
+        <v>42445</v>
       </c>
       <c r="T15" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M15,Trigger),"--")</f>
-        <v>42507</v>
+        <v>42537</v>
       </c>
       <c r="V15" s="3" t="str">
         <f t="shared" si="1"/>
@@ -3290,11 +3291,11 @@
       </c>
       <c r="Y15" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W15,Trigger),"")</f>
-        <v>1.2641861312049179E-2</v>
+        <v>1.3112351695149727E-2</v>
       </c>
       <c r="Z15" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W15)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W15)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W15)),_xll.qlSwapRateHelperSpread($W15))</f>
-        <v>8.3138687950917617E-5</v>
+        <v>6.2648304850209015E-5</v>
       </c>
       <c r="AA15" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W15,Trigger),"")</f>
@@ -3305,7 +3306,7 @@
         <v>42901</v>
       </c>
       <c r="AC15" s="68">
-        <v>8.1830679106953581E-3</v>
+        <v>9.1262640627129965E-3</v>
       </c>
       <c r="AH15" s="161"/>
     </row>
@@ -3318,7 +3319,7 @@
       </c>
       <c r="C16" s="61" t="str">
         <f>_xll.qlIMMNextCode(C15,B16,Trigger)</f>
-        <v>F6</v>
+        <v>G6</v>
       </c>
       <c r="D16" s="126"/>
       <c r="E16" s="126"/>
@@ -3329,11 +3330,11 @@
       </c>
       <c r="H16" s="120" t="str">
         <f t="shared" si="8"/>
-        <v>USDFUT3MF6_Quote</v>
+        <v>USDFUT3MG6_Quote</v>
       </c>
       <c r="I16" s="120" t="str">
         <f t="shared" si="9"/>
-        <v>USDFUT3MF6ConvAdj_Quote</v>
+        <v>USDFUT3MG6ConvAdj_Quote</v>
       </c>
       <c r="J16" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H16,$H$12,C16,G16,I16,Permanent,Trigger,ObjectOverwrite)</f>
@@ -3350,11 +3351,11 @@
       </c>
       <c r="N16" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M16,Trigger),"--")</f>
-        <v>USDFUT3MH6_Quote</v>
+        <v>USDFUT3MJ6_Quote</v>
       </c>
       <c r="O16" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M16,Trigger),"--")</f>
-        <v>99.392499999999998</v>
+        <v>99.259999999999991</v>
       </c>
       <c r="P16" s="98" t="b">
         <v>1</v>
@@ -3367,18 +3368,18 @@
       </c>
       <c r="S16" s="100">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M16,Trigger),"--")</f>
-        <v>42445</v>
+        <v>42480</v>
       </c>
       <c r="T16" s="100">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M16,Trigger),"--")</f>
-        <v>42537</v>
+        <v>42571</v>
       </c>
       <c r="V16" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Sw</v>
       </c>
       <c r="W16" s="3" t="str">
-        <v>obj_00301</v>
+        <v>obj_00307</v>
       </c>
       <c r="X16" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W16,Trigger),"")</f>
@@ -3386,7 +3387,7 @@
       </c>
       <c r="Y16" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W16,Trigger),"")</f>
-        <v>9.4699999999999993E-3</v>
+        <v>1.0449999999999999E-2</v>
       </c>
       <c r="Z16" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W16)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W16)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W16)),_xll.qlSwapRateHelperSpread($W16))</f>
@@ -3394,14 +3395,14 @@
       </c>
       <c r="AA16" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W16,Trigger),"")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="AB16" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W16,Trigger),"")</f>
-        <v>43052</v>
+        <v>43080</v>
       </c>
       <c r="AC16" s="68">
-        <v>9.5447881453849231E-3</v>
+        <v>1.0534282689287222E-2</v>
       </c>
       <c r="AH16" s="161"/>
     </row>
@@ -3414,7 +3415,7 @@
       </c>
       <c r="C17" s="61" t="str">
         <f>_xll.qlIMMNextCode(C16,B17,Trigger)</f>
-        <v>G6</v>
+        <v>H6</v>
       </c>
       <c r="D17" s="126"/>
       <c r="E17" s="126"/>
@@ -3425,11 +3426,11 @@
       </c>
       <c r="H17" s="120" t="str">
         <f t="shared" si="8"/>
-        <v>USDFUT3MG6_Quote</v>
+        <v>USDFUT3MH6_Quote</v>
       </c>
       <c r="I17" s="120" t="str">
         <f t="shared" si="9"/>
-        <v>USDFUT3MG6ConvAdj_Quote</v>
+        <v>USDFUT3MH6ConvAdj_Quote</v>
       </c>
       <c r="J17" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H17,$H$12,C17,G17,I17,Permanent,Trigger,ObjectOverwrite)</f>
@@ -3450,7 +3451,7 @@
       </c>
       <c r="O17" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M17,Trigger),"--")</f>
-        <v>99.237499999999997</v>
+        <v>99.162499999999994</v>
       </c>
       <c r="P17" s="98" t="b">
         <v>1</v>
@@ -3474,7 +3475,7 @@
         <v>Sw</v>
       </c>
       <c r="W17" s="3" t="str">
-        <v>obj_0030e</v>
+        <v>obj_00312</v>
       </c>
       <c r="X17" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W17,Trigger),"")</f>
@@ -3482,7 +3483,7 @@
       </c>
       <c r="Y17" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W17,Trigger),"")</f>
-        <v>1.2359999999999999E-2</v>
+        <v>1.295E-2</v>
       </c>
       <c r="Z17" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W17)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W17)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W17)),_xll.qlSwapRateHelperSpread($W17))</f>
@@ -3490,14 +3491,14 @@
       </c>
       <c r="AA17" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W17,Trigger),"")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="AB17" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W17,Trigger),"")</f>
-        <v>43417</v>
+        <v>43444</v>
       </c>
       <c r="AC17" s="68">
-        <v>1.2478454077713726E-2</v>
+        <v>1.3072363135210256E-2</v>
       </c>
       <c r="AH17" s="161"/>
     </row>
@@ -3510,7 +3511,7 @@
       </c>
       <c r="C18" s="8" t="str">
         <f>_xll.qlIMMNextCode(C17,B18,Trigger)</f>
-        <v>H6</v>
+        <v>J6</v>
       </c>
       <c r="D18" s="127"/>
       <c r="E18" s="127"/>
@@ -3521,11 +3522,11 @@
       </c>
       <c r="H18" s="121" t="str">
         <f t="shared" si="8"/>
-        <v>USDFUT3MH6_Quote</v>
+        <v>USDFUT3MJ6_Quote</v>
       </c>
       <c r="I18" s="121" t="str">
         <f t="shared" si="9"/>
-        <v>USDFUT3MH6ConvAdj_Quote</v>
+        <v>USDFUT3MJ6ConvAdj_Quote</v>
       </c>
       <c r="J18" s="2" t="str">
         <f>_xll.qlFuturesRateHelper(,H18,$H$12,C18,G18,I18,Permanent,Trigger,ObjectOverwrite)</f>
@@ -3546,7 +3547,7 @@
       </c>
       <c r="O18" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M18,Trigger),"--")</f>
-        <v>99.0625</v>
+        <v>98.997500000000002</v>
       </c>
       <c r="P18" s="98" t="b">
         <v>1</v>
@@ -3570,7 +3571,7 @@
         <v>Sw</v>
       </c>
       <c r="W18" s="3" t="str">
-        <v>obj_0030d</v>
+        <v>obj_00310</v>
       </c>
       <c r="X18" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W18,Trigger),"")</f>
@@ -3578,7 +3579,7 @@
       </c>
       <c r="Y18" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W18,Trigger),"")</f>
-        <v>1.4649999999999998E-2</v>
+        <v>1.49E-2</v>
       </c>
       <c r="Z18" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W18)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W18)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W18)),_xll.qlSwapRateHelperSpread($W18))</f>
@@ -3586,14 +3587,14 @@
       </c>
       <c r="AA18" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W18,Trigger),"")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="AB18" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W18,Trigger),"")</f>
-        <v>43782</v>
+        <v>43808</v>
       </c>
       <c r="AC18" s="68">
-        <v>1.4817043325496866E-2</v>
+        <v>1.5062689675156104E-2</v>
       </c>
       <c r="AH18" s="161"/>
     </row>
@@ -3642,7 +3643,7 @@
       </c>
       <c r="O19" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M19,Trigger),"--")</f>
-        <v>98.887500000000003</v>
+        <v>98.827500000000001</v>
       </c>
       <c r="P19" s="98" t="b">
         <v>1</v>
@@ -3666,7 +3667,7 @@
         <v>Sw</v>
       </c>
       <c r="W19" s="3" t="str">
-        <v>obj_00318</v>
+        <v>obj_0030e</v>
       </c>
       <c r="X19" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W19,Trigger),"")</f>
@@ -3674,7 +3675,7 @@
       </c>
       <c r="Y19" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W19,Trigger),"")</f>
-        <v>1.6490000000000001E-2</v>
+        <v>1.6469999999999999E-2</v>
       </c>
       <c r="Z19" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W19)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W19)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W19)),_xll.qlSwapRateHelperSpread($W19))</f>
@@ -3682,14 +3683,14 @@
       </c>
       <c r="AA19" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W19,Trigger),"")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="AB19" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W19,Trigger),"")</f>
-        <v>44148</v>
+        <v>44174</v>
       </c>
       <c r="AC19" s="68">
-        <v>1.6708915107592533E-2</v>
+        <v>1.6675032384037614E-2</v>
       </c>
       <c r="AH19" s="161"/>
     </row>
@@ -3738,7 +3739,7 @@
       </c>
       <c r="O20" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M20,Trigger),"--")</f>
-        <v>98.727499999999992</v>
+        <v>98.682500000000005</v>
       </c>
       <c r="P20" s="98" t="b">
         <v>1</v>
@@ -3762,7 +3763,7 @@
         <v>Sw</v>
       </c>
       <c r="W20" s="3" t="str">
-        <v>obj_0031c</v>
+        <v>obj_00313</v>
       </c>
       <c r="X20" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W20,Trigger),"")</f>
@@ -3770,7 +3771,7 @@
       </c>
       <c r="Y20" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W20,Trigger),"")</f>
-        <v>1.805E-2</v>
+        <v>1.7819999999999999E-2</v>
       </c>
       <c r="Z20" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W20)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W20)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W20)),_xll.qlSwapRateHelperSpread($W20))</f>
@@ -3778,14 +3779,14 @@
       </c>
       <c r="AA20" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W20,Trigger),"")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="AB20" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W20,Trigger),"")</f>
-        <v>44515</v>
+        <v>44539</v>
       </c>
       <c r="AC20" s="68">
-        <v>1.8325703145799729E-2</v>
+        <v>1.8072275535611564E-2</v>
       </c>
       <c r="AH20" s="161"/>
     </row>
@@ -3834,7 +3835,7 @@
       </c>
       <c r="O21" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M21,Trigger),"--")</f>
-        <v>98.5625</v>
+        <v>98.537499999999994</v>
       </c>
       <c r="P21" s="98" t="b">
         <v>1</v>
@@ -3858,7 +3859,7 @@
         <v>Sw</v>
       </c>
       <c r="W21" s="3" t="str">
-        <v>obj_0030f</v>
+        <v>obj_0030d</v>
       </c>
       <c r="X21" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W21,Trigger),"")</f>
@@ -3866,7 +3867,7 @@
       </c>
       <c r="Y21" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W21,Trigger),"")</f>
-        <v>1.9340000000000003E-2</v>
+        <v>1.8970000000000001E-2</v>
       </c>
       <c r="Z21" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W21)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W21)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W21)),_xll.qlSwapRateHelperSpread($W21))</f>
@@ -3874,14 +3875,14 @@
       </c>
       <c r="AA21" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W21,Trigger),"")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="AB21" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W21,Trigger),"")</f>
-        <v>44879</v>
+        <v>44904</v>
       </c>
       <c r="AC21" s="68">
-        <v>1.9673709338582632E-2</v>
+        <v>1.9271890952297421E-2</v>
       </c>
       <c r="AH21" s="161"/>
     </row>
@@ -3954,7 +3955,7 @@
         <v>Sw</v>
       </c>
       <c r="W22" s="3" t="str">
-        <v>obj_00319</v>
+        <v>obj_0030f</v>
       </c>
       <c r="X22" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W22,Trigger),"")</f>
@@ -3962,7 +3963,7 @@
       </c>
       <c r="Y22" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W22,Trigger),"")</f>
-        <v>2.0400000000000001E-2</v>
+        <v>1.9969999999999998E-2</v>
       </c>
       <c r="Z22" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W22)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W22)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W22)),_xll.qlSwapRateHelperSpread($W22))</f>
@@ -3970,14 +3971,14 @@
       </c>
       <c r="AA22" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W22,Trigger),"")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="AB22" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W22,Trigger),"")</f>
-        <v>45243</v>
+        <v>45271</v>
       </c>
       <c r="AC22" s="68">
-        <v>2.0800335661726455E-2</v>
+        <v>2.0323580583190729E-2</v>
       </c>
       <c r="AH22" s="161"/>
     </row>
@@ -4026,7 +4027,7 @@
       </c>
       <c r="O23" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M23,Trigger),"--")</f>
-        <v>98.259999999999991</v>
+        <v>98.282499999999999</v>
       </c>
       <c r="P23" s="98" t="b">
         <v>1</v>
@@ -4050,7 +4051,7 @@
         <v>Sw</v>
       </c>
       <c r="W23" s="3" t="str">
-        <v>obj_00310</v>
+        <v>obj_00314</v>
       </c>
       <c r="X23" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W23,Trigger),"")</f>
@@ -4058,7 +4059,7 @@
       </c>
       <c r="Y23" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W23,Trigger),"")</f>
-        <v>2.128E-2</v>
+        <v>2.0799999999999999E-2</v>
       </c>
       <c r="Z23" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W23)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W23)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W23)),_xll.qlSwapRateHelperSpread($W23))</f>
@@ -4066,14 +4067,14 @@
       </c>
       <c r="AA23" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W23,Trigger),"")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="AB23" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W23,Trigger),"")</f>
-        <v>45609</v>
+        <v>45635</v>
       </c>
       <c r="AC23" s="68">
-        <v>2.1732711881939291E-2</v>
+        <v>2.1202889666023458E-2</v>
       </c>
       <c r="AH23" s="161"/>
     </row>
@@ -4122,7 +4123,7 @@
       </c>
       <c r="O24" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M24,Trigger),"--")</f>
-        <v>98.142499999999998</v>
+        <v>98.182500000000005</v>
       </c>
       <c r="P24" s="98" t="b">
         <v>1</v>
@@ -4146,7 +4147,7 @@
         <v>Sw</v>
       </c>
       <c r="W24" s="3" t="str">
-        <v>obj_00314</v>
+        <v>obj_00319</v>
       </c>
       <c r="X24" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W24,Trigger),"")</f>
@@ -4154,7 +4155,7 @@
       </c>
       <c r="Y24" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W24,Trigger),"")</f>
-        <v>2.2029999999999998E-2</v>
+        <v>2.1530000000000001E-2</v>
       </c>
       <c r="Z24" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W24)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W24)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W24)),_xll.qlSwapRateHelperSpread($W24))</f>
@@ -4162,14 +4163,14 @@
       </c>
       <c r="AA24" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W24,Trigger),"")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="AB24" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W24,Trigger),"")</f>
-        <v>45974</v>
+        <v>46000</v>
       </c>
       <c r="AC24" s="68">
-        <v>2.2533521489388968E-2</v>
+        <v>2.1982758354630452E-2</v>
       </c>
       <c r="AH24" s="161"/>
     </row>
@@ -4218,7 +4219,7 @@
       </c>
       <c r="O25" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M25,Trigger),"--")</f>
-        <v>98.03</v>
+        <v>98.087500000000006</v>
       </c>
       <c r="P25" s="98" t="b">
         <v>1</v>
@@ -4242,7 +4243,7 @@
         <v>Sw</v>
       </c>
       <c r="W25" s="3" t="str">
-        <v>obj_00317</v>
+        <v>obj_0031c</v>
       </c>
       <c r="X25" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W25,Trigger),"")</f>
@@ -4250,7 +4251,7 @@
       </c>
       <c r="Y25" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W25,Trigger),"")</f>
-        <v>2.3279999999999999E-2</v>
+        <v>2.2700000000000001E-2</v>
       </c>
       <c r="Z25" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W25)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W25)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W25)),_xll.qlSwapRateHelperSpread($W25))</f>
@@ -4258,14 +4259,14 @@
       </c>
       <c r="AA25" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W25,Trigger),"")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="AB25" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W25,Trigger),"")</f>
-        <v>46706</v>
+        <v>46730</v>
       </c>
       <c r="AC25" s="68">
-        <v>2.3886273671146901E-2</v>
+        <v>2.3246489665210032E-2</v>
       </c>
       <c r="AH25" s="161"/>
     </row>
@@ -4314,7 +4315,7 @@
       </c>
       <c r="O26" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M26,Trigger),"--")</f>
-        <v>97.932500000000005</v>
+        <v>98.002499999999998</v>
       </c>
       <c r="P26" s="98" t="b">
         <v>1</v>
@@ -4338,7 +4339,7 @@
         <v>Sw</v>
       </c>
       <c r="W26" s="3" t="str">
-        <v>obj_00316</v>
+        <v>obj_0031b</v>
       </c>
       <c r="X26" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W26,Trigger),"")</f>
@@ -4346,7 +4347,7 @@
       </c>
       <c r="Y26" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W26,Trigger),"")</f>
-        <v>2.452E-2</v>
+        <v>2.3889999999999998E-2</v>
       </c>
       <c r="Z26" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W26)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W26)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W26)),_xll.qlSwapRateHelperSpread($W26))</f>
@@ -4354,14 +4355,14 @@
       </c>
       <c r="AA26" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W26,Trigger),"")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="AB26" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W26,Trigger),"")</f>
-        <v>47800</v>
+        <v>47826</v>
       </c>
       <c r="AC26" s="68">
-        <v>2.524412859147766E-2</v>
+        <v>2.4548189252805858E-2</v>
       </c>
       <c r="AH26" s="161"/>
     </row>
@@ -4410,7 +4411,7 @@
       </c>
       <c r="O27" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M27,Trigger),"--")</f>
-        <v>97.837500000000006</v>
+        <v>97.917500000000004</v>
       </c>
       <c r="P27" s="98" t="b">
         <v>1</v>
@@ -4434,7 +4435,7 @@
         <v>Sw</v>
       </c>
       <c r="W27" s="3" t="str">
-        <v>obj_00311</v>
+        <v>obj_00317</v>
       </c>
       <c r="X27" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W27,Trigger),"")</f>
@@ -4442,7 +4443,7 @@
       </c>
       <c r="Y27" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W27,Trigger),"")</f>
-        <v>2.5770000000000001E-2</v>
+        <v>2.5020000000000001E-2</v>
       </c>
       <c r="Z27" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W27)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W27)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W27)),_xll.qlSwapRateHelperSpread($W27))</f>
@@ -4450,14 +4451,14 @@
       </c>
       <c r="AA27" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W27,Trigger),"")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="AB27" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W27,Trigger),"")</f>
-        <v>49626</v>
+        <v>49653</v>
       </c>
       <c r="AC27" s="68">
-        <v>2.664067938956842E-2</v>
+        <v>2.5798811010566601E-2</v>
       </c>
       <c r="AH27" s="161"/>
     </row>
@@ -4506,7 +4507,7 @@
       </c>
       <c r="O28" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M28,Trigger),"--")</f>
-        <v>97.759999999999991</v>
+        <v>97.852499999999992</v>
       </c>
       <c r="P28" s="98" t="b">
         <v>1</v>
@@ -4530,7 +4531,7 @@
         <v>Sw</v>
       </c>
       <c r="W28" s="3" t="str">
-        <v>obj_00313</v>
+        <v>obj_00311</v>
       </c>
       <c r="X28" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W28,Trigger),"")</f>
@@ -4538,7 +4539,7 @@
       </c>
       <c r="Y28" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W28,Trigger),"")</f>
-        <v>2.6309999999999997E-2</v>
+        <v>2.5559999999999999E-2</v>
       </c>
       <c r="Z28" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W28)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W28)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W28)),_xll.qlSwapRateHelperSpread($W28))</f>
@@ -4546,14 +4547,14 @@
       </c>
       <c r="AA28" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W28,Trigger),"")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="AB28" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W28,Trigger),"")</f>
-        <v>51453</v>
+        <v>51480</v>
       </c>
       <c r="AC28" s="68">
-        <v>2.7194336839467616E-2</v>
+        <v>2.6376376453621959E-2</v>
       </c>
       <c r="AH28" s="161"/>
     </row>
@@ -4602,7 +4603,7 @@
       </c>
       <c r="O29" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M29,Trigger),"--")</f>
-        <v>97.682500000000005</v>
+        <v>97.782499999999999</v>
       </c>
       <c r="P29" s="98" t="b">
         <v>1</v>
@@ -4626,7 +4627,7 @@
         <v>Sw</v>
       </c>
       <c r="W29" s="3" t="str">
-        <v>obj_0031b</v>
+        <v>obj_00318</v>
       </c>
       <c r="X29" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W29,Trigger),"")</f>
@@ -4634,7 +4635,7 @@
       </c>
       <c r="Y29" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W29,Trigger),"")</f>
-        <v>2.6619999999999998E-2</v>
+        <v>2.588E-2</v>
       </c>
       <c r="Z29" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W29)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W29)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W29)),_xll.qlSwapRateHelperSpread($W29))</f>
@@ -4642,14 +4643,14 @@
       </c>
       <c r="AA29" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W29,Trigger),"")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="AB29" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W29,Trigger),"")</f>
-        <v>53279</v>
+        <v>53307</v>
       </c>
       <c r="AC29" s="68">
-        <v>2.7507350218453085E-2</v>
+        <v>2.6711010111697849E-2</v>
       </c>
       <c r="AH29" s="161"/>
     </row>
@@ -4698,7 +4699,7 @@
       </c>
       <c r="O30" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M30,Trigger),"--")</f>
-        <v>97.61</v>
+        <v>97.717500000000001</v>
       </c>
       <c r="P30" s="98" t="b">
         <v>1</v>
@@ -4722,7 +4723,7 @@
         <v>Sw</v>
       </c>
       <c r="W30" s="3" t="str">
-        <v>obj_00312</v>
+        <v>obj_00315</v>
       </c>
       <c r="X30" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W30,Trigger),"")</f>
@@ -4730,7 +4731,7 @@
       </c>
       <c r="Y30" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W30,Trigger),"")</f>
-        <v>2.6789999999999998E-2</v>
+        <v>2.6080000000000002E-2</v>
       </c>
       <c r="Z30" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W30)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W30)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W30)),_xll.qlSwapRateHelperSpread($W30))</f>
@@ -4738,14 +4739,14 @@
       </c>
       <c r="AA30" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W30,Trigger),"")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="AB30" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W30,Trigger),"")</f>
-        <v>56933</v>
+        <v>56957</v>
       </c>
       <c r="AC30" s="68">
-        <v>2.7578731092807302E-2</v>
+        <v>2.6827048606829367E-2</v>
       </c>
       <c r="AH30" s="161"/>
     </row>
@@ -4794,7 +4795,7 @@
       </c>
       <c r="O31" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M31,Trigger),"--")</f>
-        <v>97.537499999999994</v>
+        <v>97.652500000000003</v>
       </c>
       <c r="P31" s="98" t="b">
         <v>1</v>
@@ -4818,7 +4819,7 @@
         <v>Sw</v>
       </c>
       <c r="W31" s="3" t="str">
-        <v>obj_0031a</v>
+        <v>obj_00316</v>
       </c>
       <c r="X31" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W31,Trigger),"")</f>
@@ -4826,7 +4827,7 @@
       </c>
       <c r="Y31" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W31,Trigger),"")</f>
-        <v>2.6670000000000003E-2</v>
+        <v>2.5929999999999998E-2</v>
       </c>
       <c r="Z31" s="105">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W31)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W31)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W31)),_xll.qlSwapRateHelperSpread($W31))</f>
@@ -4834,14 +4835,14 @@
       </c>
       <c r="AA31" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W31,Trigger),"")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="AB31" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W31,Trigger),"")</f>
-        <v>60584</v>
+        <v>60610</v>
       </c>
       <c r="AC31" s="68">
-        <v>2.7177161234110167E-2</v>
+        <v>2.6401281946514196E-2</v>
       </c>
       <c r="AH31" s="161"/>
     </row>
@@ -4890,7 +4891,7 @@
       </c>
       <c r="O32" s="153">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M32,Trigger),"--")</f>
-        <v>97.472499999999997</v>
+        <v>97.597499999999997</v>
       </c>
       <c r="P32" s="98" t="b">
         <v>1</v>
@@ -4985,7 +4986,7 @@
       </c>
       <c r="O33" s="154">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M33,Trigger),"--")</f>
-        <v>97.407499999999999</v>
+        <v>97.537499999999994</v>
       </c>
       <c r="P33" s="101" t="b">
         <v>1</v>
@@ -5431,7 +5432,7 @@
       </c>
       <c r="M38" s="142" t="str">
         <f t="shared" si="11"/>
-        <v>obj_00301#0001</v>
+        <v>obj_00307#0001</v>
       </c>
       <c r="N38" s="151" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M38,Trigger),"--")</f>
@@ -5439,7 +5440,7 @@
       </c>
       <c r="O38" s="144">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M38,Trigger),"--")</f>
-        <v>9.4699999999999993E-3</v>
+        <v>1.0449999999999999E-2</v>
       </c>
       <c r="P38" s="143" t="b">
         <v>1</v>
@@ -5452,11 +5453,11 @@
       </c>
       <c r="S38" s="145">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M38,Trigger),"--")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="T38" s="145">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M38,Trigger),"--")</f>
-        <v>43052</v>
+        <v>43080</v>
       </c>
       <c r="V38" s="3" t="str">
         <f t="shared" si="12"/>
@@ -5527,7 +5528,7 @@
       </c>
       <c r="M39" s="142" t="str">
         <f t="shared" si="11"/>
-        <v>obj_0030e#0001</v>
+        <v>obj_00312#0001</v>
       </c>
       <c r="N39" s="151" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M39,Trigger),"--")</f>
@@ -5535,7 +5536,7 @@
       </c>
       <c r="O39" s="144">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M39,Trigger),"--")</f>
-        <v>1.2359999999999999E-2</v>
+        <v>1.295E-2</v>
       </c>
       <c r="P39" s="143" t="b">
         <v>1</v>
@@ -5548,11 +5549,11 @@
       </c>
       <c r="S39" s="145">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M39,Trigger),"--")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="T39" s="145">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M39,Trigger),"--")</f>
-        <v>43417</v>
+        <v>43444</v>
       </c>
       <c r="V39" s="3" t="str">
         <f t="shared" si="12"/>
@@ -5623,7 +5624,7 @@
       </c>
       <c r="M40" s="142" t="str">
         <f t="shared" si="11"/>
-        <v>obj_0030d#0001</v>
+        <v>obj_00310#0001</v>
       </c>
       <c r="N40" s="151" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M40,Trigger),"--")</f>
@@ -5631,7 +5632,7 @@
       </c>
       <c r="O40" s="144">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M40,Trigger),"--")</f>
-        <v>1.4649999999999998E-2</v>
+        <v>1.49E-2</v>
       </c>
       <c r="P40" s="143" t="b">
         <v>1</v>
@@ -5644,11 +5645,11 @@
       </c>
       <c r="S40" s="145">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M40,Trigger),"--")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="T40" s="145">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M40,Trigger),"--")</f>
-        <v>43782</v>
+        <v>43808</v>
       </c>
       <c r="V40" s="3" t="str">
         <f t="shared" si="12"/>
@@ -5718,7 +5719,7 @@
       </c>
       <c r="M41" s="142" t="str">
         <f t="shared" si="11"/>
-        <v>obj_00318#0001</v>
+        <v>obj_0030e#0001</v>
       </c>
       <c r="N41" s="151" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M41,Trigger),"--")</f>
@@ -5726,7 +5727,7 @@
       </c>
       <c r="O41" s="144">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M41,Trigger),"--")</f>
-        <v>1.6490000000000001E-2</v>
+        <v>1.6469999999999999E-2</v>
       </c>
       <c r="P41" s="143" t="b">
         <v>1</v>
@@ -5739,11 +5740,11 @@
       </c>
       <c r="S41" s="145">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M41,Trigger),"--")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="T41" s="145">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M41,Trigger),"--")</f>
-        <v>44148</v>
+        <v>44174</v>
       </c>
       <c r="V41" s="3" t="str">
         <f t="shared" si="12"/>
@@ -5808,7 +5809,7 @@
       </c>
       <c r="J42" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H42,,B42,JoinCalendar,USDSTD!D42,USDSTD!E42,USDSTD!F42,USDSTD!G42,USDSTD!I42,USDSTD!C42,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00301#0001</v>
+        <v>obj_00307#0001</v>
       </c>
       <c r="L42" s="69" t="str">
         <f t="shared" si="10"/>
@@ -5816,7 +5817,7 @@
       </c>
       <c r="M42" s="142" t="str">
         <f t="shared" si="11"/>
-        <v>obj_0031c#0001</v>
+        <v>obj_00313#0001</v>
       </c>
       <c r="N42" s="151" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M42,Trigger),"--")</f>
@@ -5824,7 +5825,7 @@
       </c>
       <c r="O42" s="144">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M42,Trigger),"--")</f>
-        <v>1.805E-2</v>
+        <v>1.7819999999999999E-2</v>
       </c>
       <c r="P42" s="143" t="b">
         <v>1</v>
@@ -5837,11 +5838,11 @@
       </c>
       <c r="S42" s="145">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M42,Trigger),"--")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="T42" s="145">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M42,Trigger),"--")</f>
-        <v>44515</v>
+        <v>44539</v>
       </c>
       <c r="V42" s="3" t="str">
         <f t="shared" si="12"/>
@@ -5906,7 +5907,7 @@
       </c>
       <c r="J43" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H43,,B43,JoinCalendar,USDSTD!D43,USDSTD!E43,USDSTD!F43,USDSTD!G43,USDSTD!I43,USDSTD!C43,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0030e#0001</v>
+        <v>obj_00312#0001</v>
       </c>
       <c r="L43" s="69" t="str">
         <f t="shared" si="10"/>
@@ -5914,7 +5915,7 @@
       </c>
       <c r="M43" s="142" t="str">
         <f t="shared" si="11"/>
-        <v>obj_0030f#0001</v>
+        <v>obj_0030d#0001</v>
       </c>
       <c r="N43" s="151" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M43,Trigger),"--")</f>
@@ -5922,7 +5923,7 @@
       </c>
       <c r="O43" s="144">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M43,Trigger),"--")</f>
-        <v>1.9340000000000003E-2</v>
+        <v>1.8970000000000001E-2</v>
       </c>
       <c r="P43" s="143" t="b">
         <v>1</v>
@@ -5935,11 +5936,11 @@
       </c>
       <c r="S43" s="145">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M43,Trigger),"--")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="T43" s="145">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M43,Trigger),"--")</f>
-        <v>44879</v>
+        <v>44904</v>
       </c>
       <c r="V43" s="3" t="str">
         <f t="shared" si="12"/>
@@ -6004,7 +6005,7 @@
       </c>
       <c r="J44" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H44,,B44,JoinCalendar,USDSTD!D44,USDSTD!E44,USDSTD!F44,USDSTD!G44,USDSTD!I44,USDSTD!C44,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0030d#0001</v>
+        <v>obj_00310#0001</v>
       </c>
       <c r="L44" s="69" t="str">
         <f t="shared" si="10"/>
@@ -6012,7 +6013,7 @@
       </c>
       <c r="M44" s="142" t="str">
         <f t="shared" si="11"/>
-        <v>obj_00319#0001</v>
+        <v>obj_0030f#0001</v>
       </c>
       <c r="N44" s="151" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M44,Trigger),"--")</f>
@@ -6020,7 +6021,7 @@
       </c>
       <c r="O44" s="144">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M44,Trigger),"--")</f>
-        <v>2.0400000000000001E-2</v>
+        <v>1.9969999999999998E-2</v>
       </c>
       <c r="P44" s="143" t="b">
         <v>1</v>
@@ -6033,11 +6034,11 @@
       </c>
       <c r="S44" s="145">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M44,Trigger),"--")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="T44" s="145">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M44,Trigger),"--")</f>
-        <v>45243</v>
+        <v>45271</v>
       </c>
       <c r="V44" s="3" t="str">
         <f t="shared" si="12"/>
@@ -6102,7 +6103,7 @@
       </c>
       <c r="J45" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H45,,B45,JoinCalendar,USDSTD!D45,USDSTD!E45,USDSTD!F45,USDSTD!G45,USDSTD!I45,USDSTD!C45,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00318#0001</v>
+        <v>obj_0030e#0001</v>
       </c>
       <c r="L45" s="69" t="str">
         <f t="shared" si="10"/>
@@ -6110,7 +6111,7 @@
       </c>
       <c r="M45" s="142" t="str">
         <f t="shared" si="11"/>
-        <v>obj_00310#0001</v>
+        <v>obj_00314#0001</v>
       </c>
       <c r="N45" s="151" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M45,Trigger),"--")</f>
@@ -6118,7 +6119,7 @@
       </c>
       <c r="O45" s="144">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M45,Trigger),"--")</f>
-        <v>2.128E-2</v>
+        <v>2.0799999999999999E-2</v>
       </c>
       <c r="P45" s="143" t="b">
         <v>1</v>
@@ -6131,11 +6132,11 @@
       </c>
       <c r="S45" s="145">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M45,Trigger),"--")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="T45" s="145">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M45,Trigger),"--")</f>
-        <v>45609</v>
+        <v>45635</v>
       </c>
       <c r="V45" s="3" t="str">
         <f t="shared" si="12"/>
@@ -6200,7 +6201,7 @@
       </c>
       <c r="J46" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H46,,B46,JoinCalendar,USDSTD!D46,USDSTD!E46,USDSTD!F46,USDSTD!G46,USDSTD!I46,USDSTD!C46,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0031c#0001</v>
+        <v>obj_00313#0001</v>
       </c>
       <c r="L46" s="69" t="str">
         <f t="shared" si="10"/>
@@ -6208,7 +6209,7 @@
       </c>
       <c r="M46" s="142" t="str">
         <f t="shared" si="11"/>
-        <v>obj_00314#0001</v>
+        <v>obj_00319#0001</v>
       </c>
       <c r="N46" s="151" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M46,Trigger),"--")</f>
@@ -6216,7 +6217,7 @@
       </c>
       <c r="O46" s="144">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M46,Trigger),"--")</f>
-        <v>2.2029999999999998E-2</v>
+        <v>2.1530000000000001E-2</v>
       </c>
       <c r="P46" s="143" t="b">
         <v>1</v>
@@ -6229,11 +6230,11 @@
       </c>
       <c r="S46" s="145">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M46,Trigger),"--")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="T46" s="145">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M46,Trigger),"--")</f>
-        <v>45974</v>
+        <v>46000</v>
       </c>
       <c r="V46" s="3" t="str">
         <f t="shared" si="12"/>
@@ -6298,7 +6299,7 @@
       </c>
       <c r="J47" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H47,,B47,JoinCalendar,USDSTD!D47,USDSTD!E47,USDSTD!F47,USDSTD!G47,USDSTD!I47,USDSTD!C47,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0030f#0001</v>
+        <v>obj_0030d#0001</v>
       </c>
       <c r="L47" s="69" t="str">
         <f t="shared" si="10"/>
@@ -6396,7 +6397,7 @@
       </c>
       <c r="J48" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H48,,B48,JoinCalendar,USDSTD!D48,USDSTD!E48,USDSTD!F48,USDSTD!G48,USDSTD!I48,USDSTD!C48,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00319#0001</v>
+        <v>obj_0030f#0001</v>
       </c>
       <c r="L48" s="69" t="str">
         <f t="shared" si="10"/>
@@ -6404,7 +6405,7 @@
       </c>
       <c r="M48" s="143" t="str">
         <f t="shared" si="11"/>
-        <v>obj_00317#0001</v>
+        <v>obj_0031c#0001</v>
       </c>
       <c r="N48" s="151" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M48,Trigger),"--")</f>
@@ -6412,7 +6413,7 @@
       </c>
       <c r="O48" s="144">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M48,Trigger),"--")</f>
-        <v>2.3279999999999999E-2</v>
+        <v>2.2700000000000001E-2</v>
       </c>
       <c r="P48" s="143" t="b">
         <v>1</v>
@@ -6425,11 +6426,11 @@
       </c>
       <c r="S48" s="145">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M48,Trigger),"--")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="T48" s="145">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M48,Trigger),"--")</f>
-        <v>46706</v>
+        <v>46730</v>
       </c>
       <c r="V48" s="3" t="str">
         <f t="shared" si="12"/>
@@ -6494,7 +6495,7 @@
       </c>
       <c r="J49" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H49,,B49,JoinCalendar,USDSTD!D49,USDSTD!E49,USDSTD!F49,USDSTD!G49,USDSTD!I49,USDSTD!C49,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00310#0001</v>
+        <v>obj_00314#0001</v>
       </c>
       <c r="L49" s="69" t="str">
         <f t="shared" si="10"/>
@@ -6592,7 +6593,7 @@
       </c>
       <c r="J50" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H50,,B50,JoinCalendar,USDSTD!D50,USDSTD!E50,USDSTD!F50,USDSTD!G50,USDSTD!I50,USDSTD!C50,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00314#0001</v>
+        <v>obj_00319#0001</v>
       </c>
       <c r="L50" s="69" t="str">
         <f t="shared" si="10"/>
@@ -6695,7 +6696,7 @@
       </c>
       <c r="M51" s="143" t="str">
         <f t="shared" si="11"/>
-        <v>obj_00316#0001</v>
+        <v>obj_0031b#0001</v>
       </c>
       <c r="N51" s="151" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M51,Trigger),"--")</f>
@@ -6703,7 +6704,7 @@
       </c>
       <c r="O51" s="144">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M51,Trigger),"--")</f>
-        <v>2.452E-2</v>
+        <v>2.3889999999999998E-2</v>
       </c>
       <c r="P51" s="143" t="b">
         <v>1</v>
@@ -6716,11 +6717,11 @@
       </c>
       <c r="S51" s="145">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M51,Trigger),"--")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="T51" s="145">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M51,Trigger),"--")</f>
-        <v>47800</v>
+        <v>47826</v>
       </c>
       <c r="V51" s="3" t="str">
         <f t="shared" si="12"/>
@@ -6785,7 +6786,7 @@
       </c>
       <c r="J52" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H52,,B52,JoinCalendar,USDSTD!D52,USDSTD!E52,USDSTD!F52,USDSTD!G52,USDSTD!I52,USDSTD!C52,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00317#0001</v>
+        <v>obj_0031c#0001</v>
       </c>
       <c r="L52" s="69" t="str">
         <f t="shared" si="10"/>
@@ -7073,7 +7074,7 @@
       </c>
       <c r="J55" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H55,,B55,JoinCalendar,USDSTD!D55,USDSTD!E55,USDSTD!F55,USDSTD!G55,USDSTD!I55,USDSTD!C55,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00316#0001</v>
+        <v>obj_0031b#0001</v>
       </c>
       <c r="L55" s="69" t="str">
         <f t="shared" si="10"/>
@@ -7176,7 +7177,7 @@
       </c>
       <c r="M56" s="143" t="str">
         <f t="shared" si="11"/>
-        <v>obj_00311#0001</v>
+        <v>obj_00317#0001</v>
       </c>
       <c r="N56" s="151" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M56,Trigger),"--")</f>
@@ -7184,7 +7185,7 @@
       </c>
       <c r="O56" s="144">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M56,Trigger),"--")</f>
-        <v>2.5770000000000001E-2</v>
+        <v>2.5020000000000001E-2</v>
       </c>
       <c r="P56" s="143" t="b">
         <v>1</v>
@@ -7197,11 +7198,11 @@
       </c>
       <c r="S56" s="145">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M56,Trigger),"--")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="T56" s="145">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M56,Trigger),"--")</f>
-        <v>49626</v>
+        <v>49653</v>
       </c>
       <c r="V56" s="3" t="str">
         <f t="shared" si="12"/>
@@ -7551,7 +7552,7 @@
       </c>
       <c r="J60" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H60,,B60,JoinCalendar,USDSTD!D60,USDSTD!E60,USDSTD!F60,USDSTD!G60,USDSTD!I60,USDSTD!C60,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00311#0001</v>
+        <v>obj_00317#0001</v>
       </c>
       <c r="L60" s="69" t="str">
         <f t="shared" si="10"/>
@@ -7654,7 +7655,7 @@
       </c>
       <c r="M61" s="143" t="str">
         <f t="shared" si="11"/>
-        <v>obj_00313#0001</v>
+        <v>obj_00311#0001</v>
       </c>
       <c r="N61" s="151" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M61,Trigger),"--")</f>
@@ -7662,7 +7663,7 @@
       </c>
       <c r="O61" s="144">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M61,Trigger),"--")</f>
-        <v>2.6309999999999997E-2</v>
+        <v>2.5559999999999999E-2</v>
       </c>
       <c r="P61" s="143" t="b">
         <v>1</v>
@@ -7675,11 +7676,11 @@
       </c>
       <c r="S61" s="145">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M61,Trigger),"--")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="T61" s="145">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M61,Trigger),"--")</f>
-        <v>51453</v>
+        <v>51480</v>
       </c>
       <c r="V61" s="3" t="str">
         <f t="shared" si="12"/>
@@ -8029,7 +8030,7 @@
       </c>
       <c r="J65" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H65,,B65,JoinCalendar,USDSTD!D65,USDSTD!E65,USDSTD!F65,USDSTD!G65,USDSTD!I65,USDSTD!C65,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00313#0001</v>
+        <v>obj_00311#0001</v>
       </c>
       <c r="L65" s="69" t="str">
         <f t="shared" si="10"/>
@@ -8132,7 +8133,7 @@
       </c>
       <c r="M66" s="143" t="str">
         <f t="shared" si="11"/>
-        <v>obj_0031b#0001</v>
+        <v>obj_00318#0001</v>
       </c>
       <c r="N66" s="151" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M66,Trigger),"--")</f>
@@ -8140,7 +8141,7 @@
       </c>
       <c r="O66" s="144">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M66,Trigger),"--")</f>
-        <v>2.6619999999999998E-2</v>
+        <v>2.588E-2</v>
       </c>
       <c r="P66" s="143" t="b">
         <v>1</v>
@@ -8153,11 +8154,11 @@
       </c>
       <c r="S66" s="145">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M66,Trigger),"--")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="T66" s="145">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M66,Trigger),"--")</f>
-        <v>53279</v>
+        <v>53307</v>
       </c>
       <c r="V66" s="3" t="str">
         <f t="shared" si="12"/>
@@ -8322,7 +8323,7 @@
       </c>
       <c r="M68" s="143" t="str">
         <f t="shared" si="11"/>
-        <v>obj_00312#0001</v>
+        <v>obj_00315#0001</v>
       </c>
       <c r="N68" s="151" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M68,Trigger),"--")</f>
@@ -8330,7 +8331,7 @@
       </c>
       <c r="O68" s="144">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M68,Trigger),"--")</f>
-        <v>2.6789999999999998E-2</v>
+        <v>2.6080000000000002E-2</v>
       </c>
       <c r="P68" s="163" t="b">
         <f>NOT(ISERROR(_xll.qlQuoteValue(N68)))</f>
@@ -8344,11 +8345,11 @@
       </c>
       <c r="S68" s="145">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M68,Trigger),"--")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="T68" s="145">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M68,Trigger),"--")</f>
-        <v>56933</v>
+        <v>56957</v>
       </c>
       <c r="V68" s="3" t="str">
         <f t="shared" si="12"/>
@@ -8508,7 +8509,7 @@
       </c>
       <c r="J70" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H70,,B70,JoinCalendar,USDSTD!D70,USDSTD!E70,USDSTD!F70,USDSTD!G70,USDSTD!I70,USDSTD!C70,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0031b#0001</v>
+        <v>obj_00318#0001</v>
       </c>
       <c r="L70" s="69" t="str">
         <f t="shared" si="10"/>
@@ -8516,7 +8517,7 @@
       </c>
       <c r="M70" s="143" t="str">
         <f t="shared" si="11"/>
-        <v>obj_0031a#0001</v>
+        <v>obj_00316#0001</v>
       </c>
       <c r="N70" s="151" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M70,Trigger),"--")</f>
@@ -8524,7 +8525,7 @@
       </c>
       <c r="O70" s="144">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M70,Trigger),"--")</f>
-        <v>2.6670000000000003E-2</v>
+        <v>2.5929999999999998E-2</v>
       </c>
       <c r="P70" s="163" t="b">
         <f>NOT(ISERROR(_xll.qlQuoteValue(N70)))</f>
@@ -8538,11 +8539,11 @@
       </c>
       <c r="S70" s="145">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M70,Trigger),"--")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="T70" s="145">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M70,Trigger),"--")</f>
-        <v>60584</v>
+        <v>60610</v>
       </c>
       <c r="V70" s="3" t="str">
         <f t="shared" si="12"/>
@@ -8612,7 +8613,7 @@
       </c>
       <c r="M71" s="146" t="str">
         <f t="shared" si="11"/>
-        <v>obj_00315#0001</v>
+        <v>obj_0031a#0001</v>
       </c>
       <c r="N71" s="156" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M71,Trigger),"--")</f>
@@ -8633,11 +8634,11 @@
       </c>
       <c r="S71" s="155">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M71,Trigger),"--")</f>
-        <v>42321</v>
+        <v>42347</v>
       </c>
       <c r="T71" s="155">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M71,Trigger),"--")</f>
-        <v>64236</v>
+        <v>64262</v>
       </c>
       <c r="V71" s="5" t="str">
         <f t="shared" si="12"/>
@@ -8702,7 +8703,7 @@
       </c>
       <c r="J72" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H72,,B72,JoinCalendar,USDSTD!D72,USDSTD!E72,USDSTD!F72,USDSTD!G72,USDSTD!I72,USDSTD!C72,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00312#0001</v>
+        <v>obj_00315#0001</v>
       </c>
     </row>
     <row r="73" spans="1:29" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8769,7 +8770,7 @@
       </c>
       <c r="J74" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H74,,B74,JoinCalendar,USDSTD!D74,USDSTD!E74,USDSTD!F74,USDSTD!G74,USDSTD!I74,USDSTD!C74,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0031a#0001</v>
+        <v>obj_00316#0001</v>
       </c>
     </row>
     <row r="75" spans="1:29" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8804,7 +8805,7 @@
       </c>
       <c r="J75" s="2" t="str">
         <f>_xll.qlSwapRateHelper2(,H75,,B75,JoinCalendar,USDSTD!D75,USDSTD!E75,USDSTD!F75,USDSTD!G75,USDSTD!I75,USDSTD!C75,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00315#0001</v>
+        <v>obj_0031a#0001</v>
       </c>
     </row>
     <row r="76" spans="1:29" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
USD STD: Extrapolation disabled
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/USD/USD_YCSTDBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/USD/USD_YCSTDBootstrapping.xlsx
@@ -540,7 +540,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="17">
+  <numFmts count="16">
+    <numFmt numFmtId="6" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
     <numFmt numFmtId="165" formatCode="0.0000%"/>
     <numFmt numFmtId="166" formatCode="0.00000%"/>
@@ -554,10 +555,8 @@
     <numFmt numFmtId="174" formatCode="_([$€-2]* #,##0.00_);_([$€-2]* \(#,##0.00\);_([$€-2]* &quot;-&quot;??_)"/>
     <numFmt numFmtId="175" formatCode="General_)"/>
     <numFmt numFmtId="176" formatCode="#,##0.0;#,##0.0"/>
-    <numFmt numFmtId="177" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
-    <numFmt numFmtId="178" formatCode="dd\-mmm\-yy"/>
-    <numFmt numFmtId="179" formatCode="0.0000"/>
-    <numFmt numFmtId="180" formatCode="0.0000E+00"/>
+    <numFmt numFmtId="177" formatCode="0.0000"/>
+    <numFmt numFmtId="178" formatCode="0.0000E+00"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -869,8 +868,8 @@
     <xf numFmtId="176" fontId="8" fillId="5" borderId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="6" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="6" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1087,7 +1086,7 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1096,7 +1095,7 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1187,7 +1186,7 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1200,7 +1199,7 @@
     <xf numFmtId="165" fontId="5" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="5" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="5" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1212,7 +1211,7 @@
     <xf numFmtId="165" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1223,16 +1222,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1246,7 +1245,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="180" fontId="5" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="178" fontId="5" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="172" fontId="3" fillId="10" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1889,8 +1888,7 @@
         <v>116</v>
       </c>
       <c r="D25" s="37" t="b">
-        <f>_xll.qlExtrapolatorEnableExtrapolation(YieldCurve_STD,TRUE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25" s="42"/>
     </row>

</xml_diff>